<commit_message>
Update Week 4-5 reports and add new content
</commit_message>
<xml_diff>
--- a/assets/Content/INFS603_Lit_review_anlaysis.xlsx
+++ b/assets/Content/INFS603_Lit_review_anlaysis.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/admin/Downloads/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/admin/Library/Mobile Documents/com~apple~CloudDocs/Github/Portfolio/assets/Content/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B3F54DA8-F469-E741-8D22-A522C479E7A5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2FA76432-8780-CB44-8136-3B8B420F2012}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-51040" yWindow="660" windowWidth="50880" windowHeight="20780" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-38500" yWindow="640" windowWidth="45340" windowHeight="19400" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Theme 1" sheetId="1" r:id="rId1"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="455" uniqueCount="359">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="470" uniqueCount="373">
   <si>
     <t>HCI &amp; Conversational Agents/Intelligent Systems (Older Adults) - Focus: Older adults interacting with AI systems, voice assistants, chatbots. Keywords: trust-building, interaction patterns, conversational AI</t>
   </si>
@@ -1685,12 +1685,62 @@
   <si>
     <t>Canada - National AI ecosystem; Three institutes: Amii (Edmonton), Mila (Montréal), Vector Institute (Toronto); policy-makers, industry partners, researchers, students nationwide</t>
   </si>
+  <si>
+    <t>Infocomm Media Development Authority (IMDA). (2024). Model AI Governance Framework for GenAI and Agentic AI Systems (2nd ed.). Singapore: Infocomm Media Development Authority.</t>
+  </si>
+  <si>
+    <t>IMDA</t>
+  </si>
+  <si>
+    <t>Framework / Model Governance Guidance（non‑binding policy）</t>
+  </si>
+  <si>
+    <t>https://www.imda.gov.sg/resources/ai-governance/Model-AI-Governance-Framework</t>
+  </si>
+  <si>
+    <t>How can organizations govern and manage risks of GenAI and agentic AI systems—especially autonomy, safety, accountability and human oversight—throughout design, deployment and operation?</t>
+  </si>
+  <si>
+    <t>N/A（policy / framework document)</t>
+  </si>
+  <si>
+    <t>Organizations and practitioners developing, deploying or using GenAI / agentic AI systems in Singapore and globally</t>
+  </si>
+  <si>
+    <t>Model governance framework / guidance that builds on the original Model AI Governance Framework and AIGC guidelines, revised using pilot project experience, public consultation, and industry collaboration.</t>
+  </si>
+  <si>
+    <t>Agentic AI risk dimensions (e.g., autonomous actions, goal alignment, predictability).
+Organizational governance structures and allocation of responsibilities (board, management, technical teams).
+Risk-control activities across the AI lifecycle: pre‑design, training, deployment, operation, and decommissioning.
+Key practical recommendations: human‑in‑the‑loop / human‑over‑the‑loop, risk assessment, incident reporting, third‑party / supply‑chain governance.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The IMDA Model Governance Framework proposes a practice‑oriented governance architecture for GenAI and agentic AI systems, emphasizing:
+(1) operationalizing existing AI principles (e.g., transparency, fairness, accountability) into concrete governance processes and control points (such as role allocation, review and oversight mechanisms);
+(2) introducing additional safeguards for agentic AI’s autonomous actions and long‑running behavior (continuous monitoring, kill‑switch / override mechanisms, and mandated human intervention);
+(3) using organization‑level risk management, supply‑chain oversight, and record‑keeping to enable traceability and accountability for AI system behavior. The framework is positioned as a voluntary, technology‑ and sector‑neutral reference, not a legally binding regulation.
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The framework is an official guideline for a single jurisdiction (Singapore) but is designed to be exportable and encourages cross‑border and cross‑industry adoption. It is compatible with international frameworks such as WHO and NIST, and places particular emphasis on human involvement, proportional risk management, and concrete practice examples (e.g., use‑case checklists) in agentic AI scenarios. A key limitation is that it does not set explicit thresholds for “acceptable risk”, so the depth of implementation depends on each organization’s internal governance capacity.
+</t>
+  </si>
+  <si>
+    <t>N/A (not an empirical study; consensus document based on policy analysis, expert consultation, and pilot experiences).</t>
+  </si>
+  <si>
+    <t>Singapore</t>
+  </si>
+  <si>
+    <t>Government / regulator publication – Infocomm Media Development Authority (IMDA), Singapore Government.</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="11" x14ac:knownFonts="1">
+  <fonts count="12" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1756,8 +1806,14 @@
       <color theme="1"/>
       <name val="Aptos Narrow (Body)"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Aptos Narrow"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="9">
+  <fills count="10">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1800,8 +1856,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="1"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="6">
+  <borders count="7">
     <border>
       <left/>
       <right/>
@@ -1872,12 +1934,25 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="123">
+  <cellXfs count="133">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -2002,6 +2077,204 @@
     <xf numFmtId="0" fontId="5" fillId="7" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="2" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="2" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="2" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="8" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="2" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="7" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="7" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="7" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="7" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="8" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="7" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="7" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="2" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="2" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="2" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="2" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -2020,230 +2293,62 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="9" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="9" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="6" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="7" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="7" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="2" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="2" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="2" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="8" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="2" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="7" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="6" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="7" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="7" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="7" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="7" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="8" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="7" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="7" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="2" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="2" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="2" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="2" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -2252,6 +2357,57 @@
   </cellStyles>
   <dxfs count="72">
     <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border outline="0">
+        <left style="thin">
+          <color rgb="FF000000"/>
+        </left>
+        <right style="thin">
+          <color rgb="FF000000"/>
+        </right>
+        <top style="thin">
+          <color rgb="FF000000"/>
+        </top>
+        <bottom style="thin">
+          <color rgb="FF000000"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border outline="0">
+        <left style="thin">
+          <color rgb="FF000000"/>
+        </left>
+        <right style="thin">
+          <color rgb="FF000000"/>
+        </right>
+        <top style="thin">
+          <color rgb="FF000000"/>
+        </top>
+        <bottom style="thin">
+          <color rgb="FF000000"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="1" indent="0" shrinkToFit="0"/>
+      <border>
+        <left style="thin">
+          <color rgb="FF000000"/>
+        </left>
+        <right style="thin">
+          <color rgb="FF000000"/>
+        </right>
+        <top style="thin">
+          <color rgb="FF000000"/>
+        </top>
+        <bottom style="thin">
+          <color rgb="FF000000"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
       <alignment horizontal="center" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <border outline="0">
         <left style="thin">
@@ -2269,6 +2425,187 @@
       </border>
     </dxf>
     <dxf>
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="1" indent="0" shrinkToFit="0"/>
+      <border>
+        <left style="thin">
+          <color rgb="FF000000"/>
+        </left>
+        <right style="thin">
+          <color rgb="FF000000"/>
+        </right>
+        <top style="thin">
+          <color rgb="FF000000"/>
+        </top>
+        <bottom style="thin">
+          <color rgb="FF000000"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="1" indent="0" shrinkToFit="0"/>
+      <border>
+        <left style="thin">
+          <color rgb="FF000000"/>
+        </left>
+        <right style="thin">
+          <color rgb="FF000000"/>
+        </right>
+        <top style="thin">
+          <color rgb="FF000000"/>
+        </top>
+        <bottom style="thin">
+          <color rgb="FF000000"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="1" indent="0" shrinkToFit="0"/>
+      <border>
+        <left style="thin">
+          <color rgb="FF000000"/>
+        </left>
+        <right style="thin">
+          <color rgb="FF000000"/>
+        </right>
+        <top style="thin">
+          <color rgb="FF000000"/>
+        </top>
+        <bottom style="thin">
+          <color rgb="FF000000"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border outline="0">
+        <left style="thin">
+          <color rgb="FF000000"/>
+        </left>
+        <right style="thin">
+          <color rgb="FF000000"/>
+        </right>
+        <top style="thin">
+          <color rgb="FF000000"/>
+        </top>
+        <bottom style="thin">
+          <color rgb="FF000000"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="1" indent="0" shrinkToFit="0"/>
+      <border>
+        <left style="thin">
+          <color rgb="FF000000"/>
+        </left>
+        <right style="thin">
+          <color rgb="FF000000"/>
+        </right>
+        <top style="thin">
+          <color rgb="FF000000"/>
+        </top>
+        <bottom style="thin">
+          <color rgb="FF000000"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border outline="0">
+        <left style="thin">
+          <color rgb="FF000000"/>
+        </left>
+        <right style="thin">
+          <color rgb="FF000000"/>
+        </right>
+        <top style="thin">
+          <color rgb="FF000000"/>
+        </top>
+        <bottom style="thin">
+          <color rgb="FF000000"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="10"/>
+        <name val="Aptos Narrow (Body)"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border outline="0">
+        <left style="thin">
+          <color rgb="FF000000"/>
+        </left>
+        <right style="thin">
+          <color rgb="FF000000"/>
+        </right>
+        <top style="thin">
+          <color rgb="FF000000"/>
+        </top>
+        <bottom style="thin">
+          <color rgb="FF000000"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment vertical="top" textRotation="0" wrapText="0" indent="0" shrinkToFit="0"/>
+      <border>
+        <left style="thin">
+          <color rgb="FF000000"/>
+        </left>
+        <right style="thin">
+          <color rgb="FF000000"/>
+        </right>
+        <top style="thin">
+          <color rgb="FF000000"/>
+        </top>
+        <bottom style="thin">
+          <color rgb="FF000000"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border outline="0">
+        <left style="thin">
+          <color rgb="FF000000"/>
+        </left>
+        <right style="thin">
+          <color rgb="FF000000"/>
+        </right>
+        <top style="thin">
+          <color rgb="FF000000"/>
+        </top>
+        <bottom style="thin">
+          <color rgb="FF000000"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="top" textRotation="0" wrapText="0" indent="0" shrinkToFit="0"/>
+      <border>
+        <left style="thin">
+          <color rgb="FF000000"/>
+        </left>
+        <right style="thin">
+          <color rgb="FF000000"/>
+        </right>
+        <top style="thin">
+          <color rgb="FF000000"/>
+        </top>
+        <bottom style="thin">
+          <color rgb="FF000000"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <border outline="0">
         <left style="thin">
@@ -2286,6 +2623,48 @@
       </border>
     </dxf>
     <dxf>
+      <font>
+        <color theme="0" tint="-0.249977111117893"/>
+      </font>
+      <alignment vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border outline="0">
+        <left style="thin">
+          <color rgb="FF000000"/>
+        </left>
+        <right style="thin">
+          <color rgb="FF000000"/>
+        </right>
+        <top style="thin">
+          <color rgb="FF000000"/>
+        </top>
+        <bottom style="thin">
+          <color rgb="FF000000"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="top" textRotation="0" wrapText="0" indent="0" shrinkToFit="0"/>
+      <border>
+        <left style="thin">
+          <color rgb="FF000000"/>
+        </left>
+        <right style="thin">
+          <color rgb="FF000000"/>
+        </right>
+        <top style="thin">
+          <color rgb="FF000000"/>
+        </top>
+        <bottom style="thin">
+          <color rgb="FF000000"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+      </font>
+    </dxf>
+    <dxf>
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <border outline="0">
         <left style="thin">
@@ -2320,24 +2699,92 @@
       </border>
     </dxf>
     <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border outline="0">
+        <left style="thin">
+          <color rgb="FF000000"/>
+        </left>
+        <right style="thin">
+          <color rgb="FF000000"/>
+        </right>
+        <top style="thin">
+          <color rgb="FF000000"/>
+        </top>
+        <bottom style="thin">
+          <color rgb="FF000000"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border outline="0">
+        <left style="thin">
+          <color rgb="FF000000"/>
+        </left>
+        <right style="thin">
+          <color rgb="FF000000"/>
+        </right>
+        <top style="thin">
+          <color rgb="FF000000"/>
+        </top>
+        <bottom style="thin">
+          <color rgb="FF000000"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border outline="0">
+        <left style="thin">
+          <color rgb="FF000000"/>
+        </left>
+        <right style="thin">
+          <color rgb="FF000000"/>
+        </right>
+        <top style="thin">
+          <color rgb="FF000000"/>
+        </top>
+        <bottom style="thin">
+          <color rgb="FF000000"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border outline="0">
+        <left style="thin">
+          <color rgb="FF000000"/>
+        </left>
+        <right style="thin">
+          <color rgb="FF000000"/>
+        </right>
+        <top style="thin">
+          <color rgb="FF000000"/>
+        </top>
+        <bottom style="thin">
+          <color rgb="FF000000"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border outline="0">
+        <left style="thin">
+          <color rgb="FF000000"/>
+        </left>
+        <right style="thin">
+          <color rgb="FF000000"/>
+        </right>
+        <top style="thin">
+          <color rgb="FF000000"/>
+        </top>
+        <bottom style="thin">
+          <color rgb="FF000000"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
       <alignment horizontal="center" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border outline="0">
-        <left style="thin">
-          <color rgb="FF000000"/>
-        </left>
-        <right style="thin">
-          <color rgb="FF000000"/>
-        </right>
-        <top style="thin">
-          <color rgb="FF000000"/>
-        </top>
-        <bottom style="thin">
-          <color rgb="FF000000"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <border outline="0">
         <left style="thin">
           <color rgb="FF000000"/>
@@ -2416,6 +2863,23 @@
       </border>
     </dxf>
     <dxf>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border outline="0">
+        <left style="thin">
+          <color rgb="FF000000"/>
+        </left>
+        <right style="thin">
+          <color rgb="FF000000"/>
+        </right>
+        <top style="thin">
+          <color rgb="FF000000"/>
+        </top>
+        <bottom style="thin">
+          <color rgb="FF000000"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <border outline="0">
         <left style="thin">
@@ -2450,108 +2914,6 @@
       </border>
     </dxf>
     <dxf>
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border outline="0">
-        <left style="thin">
-          <color rgb="FF000000"/>
-        </left>
-        <right style="thin">
-          <color rgb="FF000000"/>
-        </right>
-        <top style="thin">
-          <color rgb="FF000000"/>
-        </top>
-        <bottom style="thin">
-          <color rgb="FF000000"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border outline="0">
-        <left style="thin">
-          <color rgb="FF000000"/>
-        </left>
-        <right style="thin">
-          <color rgb="FF000000"/>
-        </right>
-        <top style="thin">
-          <color rgb="FF000000"/>
-        </top>
-        <bottom style="thin">
-          <color rgb="FF000000"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border outline="0">
-        <left style="thin">
-          <color rgb="FF000000"/>
-        </left>
-        <right style="thin">
-          <color rgb="FF000000"/>
-        </right>
-        <top style="thin">
-          <color rgb="FF000000"/>
-        </top>
-        <bottom style="thin">
-          <color rgb="FF000000"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border outline="0">
-        <left style="thin">
-          <color rgb="FF000000"/>
-        </left>
-        <right style="thin">
-          <color rgb="FF000000"/>
-        </right>
-        <top style="thin">
-          <color rgb="FF000000"/>
-        </top>
-        <bottom style="thin">
-          <color rgb="FF000000"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border outline="0">
-        <left style="thin">
-          <color rgb="FF000000"/>
-        </left>
-        <right style="thin">
-          <color rgb="FF000000"/>
-        </right>
-        <top style="thin">
-          <color rgb="FF000000"/>
-        </top>
-        <bottom style="thin">
-          <color rgb="FF000000"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border outline="0">
-        <left style="thin">
-          <color rgb="FF000000"/>
-        </left>
-        <right style="thin">
-          <color rgb="FF000000"/>
-        </right>
-        <top style="thin">
-          <color rgb="FF000000"/>
-        </top>
-        <bottom style="thin">
-          <color rgb="FF000000"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <border outline="0">
         <left style="thin">
@@ -2569,6 +2931,48 @@
       </border>
     </dxf>
     <dxf>
+      <font>
+        <color theme="0" tint="-0.249977111117893"/>
+      </font>
+      <alignment vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border outline="0">
+        <left style="thin">
+          <color rgb="FF000000"/>
+        </left>
+        <right style="thin">
+          <color rgb="FF000000"/>
+        </right>
+        <top style="thin">
+          <color rgb="FF000000"/>
+        </top>
+        <bottom style="thin">
+          <color rgb="FF000000"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="top" textRotation="0" wrapText="0" indent="0" shrinkToFit="0"/>
+      <border>
+        <left style="thin">
+          <color rgb="FF000000"/>
+        </left>
+        <right style="thin">
+          <color rgb="FF000000"/>
+        </right>
+        <top style="thin">
+          <color rgb="FF000000"/>
+        </top>
+        <bottom style="thin">
+          <color rgb="FF000000"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+      </font>
+    </dxf>
+    <dxf>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <border outline="0">
         <left style="thin">
@@ -2586,7 +2990,143 @@
       </border>
     </dxf>
     <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border outline="0">
+        <left style="thin">
+          <color rgb="FF000000"/>
+        </left>
+        <right style="thin">
+          <color rgb="FF000000"/>
+        </right>
+        <top style="thin">
+          <color rgb="FF000000"/>
+        </top>
+        <bottom style="thin">
+          <color rgb="FF000000"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="1" indent="0" shrinkToFit="0"/>
+      <border>
+        <left style="thin">
+          <color rgb="FF000000"/>
+        </left>
+        <right style="thin">
+          <color rgb="FF000000"/>
+        </right>
+        <top style="thin">
+          <color rgb="FF000000"/>
+        </top>
+        <bottom style="thin">
+          <color rgb="FF000000"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border outline="0">
+        <left style="thin">
+          <color rgb="FF000000"/>
+        </left>
+        <right style="thin">
+          <color rgb="FF000000"/>
+        </right>
+        <top style="thin">
+          <color rgb="FF000000"/>
+        </top>
+        <bottom style="thin">
+          <color rgb="FF000000"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="1" indent="0" shrinkToFit="0"/>
+      <border>
+        <left style="thin">
+          <color rgb="FF000000"/>
+        </left>
+        <right style="thin">
+          <color rgb="FF000000"/>
+        </right>
+        <top style="thin">
+          <color rgb="FF000000"/>
+        </top>
+        <bottom style="thin">
+          <color rgb="FF000000"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="1" indent="0" shrinkToFit="0"/>
+      <border>
+        <left style="thin">
+          <color rgb="FF000000"/>
+        </left>
+        <right style="thin">
+          <color rgb="FF000000"/>
+        </right>
+        <top style="thin">
+          <color rgb="FF000000"/>
+        </top>
+        <bottom style="thin">
+          <color rgb="FF000000"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="1" indent="0" shrinkToFit="0"/>
+      <border>
+        <left style="thin">
+          <color rgb="FF000000"/>
+        </left>
+        <right style="thin">
+          <color rgb="FF000000"/>
+        </right>
+        <top style="thin">
+          <color rgb="FF000000"/>
+        </top>
+        <bottom style="thin">
+          <color rgb="FF000000"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="0" indent="0" shrinkToFit="0"/>
+      <border>
+        <left style="thin">
+          <color rgb="FF000000"/>
+        </left>
+        <right style="thin">
+          <color rgb="FF000000"/>
+        </right>
+        <top style="thin">
+          <color rgb="FF000000"/>
+        </top>
+        <bottom style="thin">
+          <color rgb="FF000000"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="1" indent="0" shrinkToFit="0"/>
+      <border>
+        <left style="thin">
+          <color rgb="FF000000"/>
+        </left>
+        <right style="thin">
+          <color rgb="FF000000"/>
+        </right>
+        <top style="thin">
+          <color rgb="FF000000"/>
+        </top>
+        <bottom style="thin">
+          <color rgb="FF000000"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <border outline="0">
         <left style="thin">
           <color rgb="FF000000"/>
@@ -2631,8 +3171,60 @@
       </border>
     </dxf>
     <dxf>
+      <alignment vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border outline="0">
+        <left style="thin">
+          <color rgb="FF000000"/>
+        </left>
+        <right style="thin">
+          <color rgb="FF000000"/>
+        </right>
+        <top style="thin">
+          <color rgb="FF000000"/>
+        </top>
+        <bottom style="thin">
+          <color rgb="FF000000"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <border outline="0">
+        <left style="thin">
+          <color rgb="FF000000"/>
+        </left>
+        <right style="thin">
+          <color rgb="FF000000"/>
+        </right>
+        <top style="thin">
+          <color rgb="FF000000"/>
+        </top>
+        <bottom style="thin">
+          <color rgb="FF000000"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <alignment horizontal="center" vertical="top" textRotation="0" wrapText="0" indent="0" shrinkToFit="0"/>
+      <border outline="0">
+        <left style="thin">
+          <color rgb="FF000000"/>
+        </left>
+        <right style="thin">
+          <color rgb="FF000000"/>
+        </right>
+        <top style="thin">
+          <color rgb="FF000000"/>
+        </top>
+        <bottom style="thin">
+          <color rgb="FF000000"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment vertical="top" textRotation="0" wrapText="0" indent="0" shrinkToFit="0"/>
+      <border>
         <left style="thin">
           <color rgb="FF000000"/>
         </left>
@@ -2668,10 +3260,182 @@
       </border>
     </dxf>
     <dxf>
+      <alignment horizontal="center" vertical="top" textRotation="0" wrapText="0" indent="0" shrinkToFit="0"/>
+      <border>
+        <left style="thin">
+          <color rgb="FF000000"/>
+        </left>
+        <right style="thin">
+          <color rgb="FF000000"/>
+        </right>
+        <top style="thin">
+          <color rgb="FF000000"/>
+        </top>
+        <bottom style="thin">
+          <color rgb="FF000000"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
       <font>
-        <color theme="0" tint="-0.249977111117893"/>
+        <b/>
       </font>
-      <alignment vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border outline="0">
+        <left style="thin">
+          <color rgb="FF000000"/>
+        </left>
+        <right style="thin">
+          <color rgb="FF000000"/>
+        </right>
+        <top style="thin">
+          <color rgb="FF000000"/>
+        </top>
+        <bottom style="thin">
+          <color rgb="FF000000"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border outline="0">
+        <left style="thin">
+          <color rgb="FF000000"/>
+        </left>
+        <right style="thin">
+          <color rgb="FF000000"/>
+        </right>
+        <top style="thin">
+          <color rgb="FF000000"/>
+        </top>
+        <bottom style="thin">
+          <color rgb="FF000000"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border outline="0">
+        <left style="thin">
+          <color rgb="FF000000"/>
+        </left>
+        <right style="thin">
+          <color rgb="FF000000"/>
+        </right>
+        <top style="thin">
+          <color rgb="FF000000"/>
+        </top>
+        <bottom style="thin">
+          <color rgb="FF000000"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border outline="0">
+        <left style="thin">
+          <color rgb="FF000000"/>
+        </left>
+        <right style="thin">
+          <color rgb="FF000000"/>
+        </right>
+        <top style="thin">
+          <color rgb="FF000000"/>
+        </top>
+        <bottom style="thin">
+          <color rgb="FF000000"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border outline="0">
+        <left style="thin">
+          <color rgb="FF000000"/>
+        </left>
+        <right style="thin">
+          <color rgb="FF000000"/>
+        </right>
+        <top style="thin">
+          <color rgb="FF000000"/>
+        </top>
+        <bottom style="thin">
+          <color rgb="FF000000"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border outline="0">
+        <left style="thin">
+          <color rgb="FF000000"/>
+        </left>
+        <right style="thin">
+          <color rgb="FF000000"/>
+        </right>
+        <top style="thin">
+          <color rgb="FF000000"/>
+        </top>
+        <bottom style="thin">
+          <color rgb="FF000000"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border outline="0">
+        <left style="thin">
+          <color rgb="FF000000"/>
+        </left>
+        <right style="thin">
+          <color rgb="FF000000"/>
+        </right>
+        <top style="thin">
+          <color rgb="FF000000"/>
+        </top>
+        <bottom style="thin">
+          <color rgb="FF000000"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border outline="0">
+        <left style="thin">
+          <color rgb="FF000000"/>
+        </left>
+        <right style="thin">
+          <color rgb="FF000000"/>
+        </right>
+        <top style="thin">
+          <color rgb="FF000000"/>
+        </top>
+        <bottom style="thin">
+          <color rgb="FF000000"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border outline="0">
+        <left style="thin">
+          <color rgb="FF000000"/>
+        </left>
+        <right style="thin">
+          <color rgb="FF000000"/>
+        </right>
+        <top style="thin">
+          <color rgb="FF000000"/>
+        </top>
+        <bottom style="thin">
+          <color rgb="FF000000"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <border outline="0">
         <left style="thin">
           <color rgb="FF000000"/>
@@ -2716,6 +3480,23 @@
       </border>
     </dxf>
     <dxf>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border outline="0">
+        <left style="thin">
+          <color rgb="FF000000"/>
+        </left>
+        <right style="thin">
+          <color rgb="FF000000"/>
+        </right>
+        <top style="thin">
+          <color rgb="FF000000"/>
+        </top>
+        <bottom style="thin">
+          <color rgb="FF000000"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
       <alignment horizontal="center" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <border outline="0">
         <left style="thin">
@@ -2733,159 +3514,8 @@
       </border>
     </dxf>
     <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="10"/>
-        <name val="Aptos Narrow (Body)"/>
-        <scheme val="minor"/>
-      </font>
-      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border outline="0">
-        <left style="thin">
-          <color rgb="FF000000"/>
-        </left>
-        <right style="thin">
-          <color rgb="FF000000"/>
-        </right>
-        <top style="thin">
-          <color rgb="FF000000"/>
-        </top>
-        <bottom style="thin">
-          <color rgb="FF000000"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border outline="0">
-        <left style="thin">
-          <color rgb="FF000000"/>
-        </left>
-        <right style="thin">
-          <color rgb="FF000000"/>
-        </right>
-        <top style="thin">
-          <color rgb="FF000000"/>
-        </top>
-        <bottom style="thin">
-          <color rgb="FF000000"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border outline="0">
-        <left style="thin">
-          <color rgb="FF000000"/>
-        </left>
-        <right style="thin">
-          <color rgb="FF000000"/>
-        </right>
-        <top style="thin">
-          <color rgb="FF000000"/>
-        </top>
-        <bottom style="thin">
-          <color rgb="FF000000"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border outline="0">
-        <left style="thin">
-          <color rgb="FF000000"/>
-        </left>
-        <right style="thin">
-          <color rgb="FF000000"/>
-        </right>
-        <top style="thin">
-          <color rgb="FF000000"/>
-        </top>
-        <bottom style="thin">
-          <color rgb="FF000000"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border outline="0">
-        <left style="thin">
-          <color rgb="FF000000"/>
-        </left>
-        <right style="thin">
-          <color rgb="FF000000"/>
-        </right>
-        <top style="thin">
-          <color rgb="FF000000"/>
-        </top>
-        <bottom style="thin">
-          <color rgb="FF000000"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-      <alignment horizontal="center" vertical="top" textRotation="0" wrapText="0" indent="0" shrinkToFit="0"/>
-      <border outline="0">
-        <left style="thin">
-          <color rgb="FF000000"/>
-        </left>
-        <right style="thin">
-          <color rgb="FF000000"/>
-        </right>
-        <top style="thin">
-          <color rgb="FF000000"/>
-        </top>
-        <bottom style="thin">
-          <color rgb="FF000000"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border outline="0">
-        <left style="thin">
-          <color rgb="FF000000"/>
-        </left>
-        <right style="thin">
-          <color rgb="FF000000"/>
-        </right>
-        <top style="thin">
-          <color rgb="FF000000"/>
-        </top>
-        <bottom style="thin">
-          <color rgb="FF000000"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <alignment vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border outline="0">
-        <left style="thin">
-          <color rgb="FF000000"/>
-        </left>
-        <right style="thin">
-          <color rgb="FF000000"/>
-        </right>
-        <top style="thin">
-          <color rgb="FF000000"/>
-        </top>
-        <bottom style="thin">
-          <color rgb="FF000000"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0" tint="-0.249977111117893"/>
-      </font>
-      <alignment vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border outline="0">
+      <alignment horizontal="center" vertical="top" textRotation="0" wrapText="1" indent="0" shrinkToFit="0"/>
+      <border>
         <left style="thin">
           <color rgb="FF000000"/>
         </left>
@@ -2903,548 +3533,6 @@
     <dxf>
       <alignment horizontal="center" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <border outline="0">
-        <left style="thin">
-          <color rgb="FF000000"/>
-        </left>
-        <right style="thin">
-          <color rgb="FF000000"/>
-        </right>
-        <top style="thin">
-          <color rgb="FF000000"/>
-        </top>
-        <bottom style="thin">
-          <color rgb="FF000000"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border outline="0">
-        <left style="thin">
-          <color rgb="FF000000"/>
-        </left>
-        <right style="thin">
-          <color rgb="FF000000"/>
-        </right>
-        <top style="thin">
-          <color rgb="FF000000"/>
-        </top>
-        <bottom style="thin">
-          <color rgb="FF000000"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border outline="0">
-        <left style="thin">
-          <color rgb="FF000000"/>
-        </left>
-        <right style="thin">
-          <color rgb="FF000000"/>
-        </right>
-        <top style="thin">
-          <color rgb="FF000000"/>
-        </top>
-        <bottom style="thin">
-          <color rgb="FF000000"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border outline="0">
-        <left style="thin">
-          <color rgb="FF000000"/>
-        </left>
-        <right style="thin">
-          <color rgb="FF000000"/>
-        </right>
-        <top style="thin">
-          <color rgb="FF000000"/>
-        </top>
-        <bottom style="thin">
-          <color rgb="FF000000"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border outline="0">
-        <left style="thin">
-          <color rgb="FF000000"/>
-        </left>
-        <right style="thin">
-          <color rgb="FF000000"/>
-        </right>
-        <top style="thin">
-          <color rgb="FF000000"/>
-        </top>
-        <bottom style="thin">
-          <color rgb="FF000000"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border outline="0">
-        <left style="thin">
-          <color rgb="FF000000"/>
-        </left>
-        <right style="thin">
-          <color rgb="FF000000"/>
-        </right>
-        <top style="thin">
-          <color rgb="FF000000"/>
-        </top>
-        <bottom style="thin">
-          <color rgb="FF000000"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border outline="0">
-        <left style="thin">
-          <color rgb="FF000000"/>
-        </left>
-        <right style="thin">
-          <color rgb="FF000000"/>
-        </right>
-        <top style="thin">
-          <color rgb="FF000000"/>
-        </top>
-        <bottom style="thin">
-          <color rgb="FF000000"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border outline="0">
-        <left style="thin">
-          <color rgb="FF000000"/>
-        </left>
-        <right style="thin">
-          <color rgb="FF000000"/>
-        </right>
-        <top style="thin">
-          <color rgb="FF000000"/>
-        </top>
-        <bottom style="thin">
-          <color rgb="FF000000"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border outline="0">
-        <left style="thin">
-          <color rgb="FF000000"/>
-        </left>
-        <right style="thin">
-          <color rgb="FF000000"/>
-        </right>
-        <top style="thin">
-          <color rgb="FF000000"/>
-        </top>
-        <bottom style="thin">
-          <color rgb="FF000000"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border outline="0">
-        <left style="thin">
-          <color rgb="FF000000"/>
-        </left>
-        <right style="thin">
-          <color rgb="FF000000"/>
-        </right>
-        <top style="thin">
-          <color rgb="FF000000"/>
-        </top>
-        <bottom style="thin">
-          <color rgb="FF000000"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border outline="0">
-        <left style="thin">
-          <color rgb="FF000000"/>
-        </left>
-        <right style="thin">
-          <color rgb="FF000000"/>
-        </right>
-        <top style="thin">
-          <color rgb="FF000000"/>
-        </top>
-        <bottom style="thin">
-          <color rgb="FF000000"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border outline="0">
-        <left style="thin">
-          <color rgb="FF000000"/>
-        </left>
-        <right style="thin">
-          <color rgb="FF000000"/>
-        </right>
-        <top style="thin">
-          <color rgb="FF000000"/>
-        </top>
-        <bottom style="thin">
-          <color rgb="FF000000"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border outline="0">
-        <left style="thin">
-          <color rgb="FF000000"/>
-        </left>
-        <right style="thin">
-          <color rgb="FF000000"/>
-        </right>
-        <top style="thin">
-          <color rgb="FF000000"/>
-        </top>
-        <bottom style="thin">
-          <color rgb="FF000000"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border outline="0">
-        <left style="thin">
-          <color rgb="FF000000"/>
-        </left>
-        <right style="thin">
-          <color rgb="FF000000"/>
-        </right>
-        <top style="thin">
-          <color rgb="FF000000"/>
-        </top>
-        <bottom style="thin">
-          <color rgb="FF000000"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="1" indent="0" shrinkToFit="0"/>
-      <border>
-        <left style="thin">
-          <color rgb="FF000000"/>
-        </left>
-        <right style="thin">
-          <color rgb="FF000000"/>
-        </right>
-        <top style="thin">
-          <color rgb="FF000000"/>
-        </top>
-        <bottom style="thin">
-          <color rgb="FF000000"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="1" indent="0" shrinkToFit="0"/>
-      <border>
-        <left style="thin">
-          <color rgb="FF000000"/>
-        </left>
-        <right style="thin">
-          <color rgb="FF000000"/>
-        </right>
-        <top style="thin">
-          <color rgb="FF000000"/>
-        </top>
-        <bottom style="thin">
-          <color rgb="FF000000"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="1" indent="0" shrinkToFit="0"/>
-      <border>
-        <left style="thin">
-          <color rgb="FF000000"/>
-        </left>
-        <right style="thin">
-          <color rgb="FF000000"/>
-        </right>
-        <top style="thin">
-          <color rgb="FF000000"/>
-        </top>
-        <bottom style="thin">
-          <color rgb="FF000000"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="1" indent="0" shrinkToFit="0"/>
-      <border>
-        <left style="thin">
-          <color rgb="FF000000"/>
-        </left>
-        <right style="thin">
-          <color rgb="FF000000"/>
-        </right>
-        <top style="thin">
-          <color rgb="FF000000"/>
-        </top>
-        <bottom style="thin">
-          <color rgb="FF000000"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="1" indent="0" shrinkToFit="0"/>
-      <border>
-        <left style="thin">
-          <color rgb="FF000000"/>
-        </left>
-        <right style="thin">
-          <color rgb="FF000000"/>
-        </right>
-        <top style="thin">
-          <color rgb="FF000000"/>
-        </top>
-        <bottom style="thin">
-          <color rgb="FF000000"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <alignment vertical="top" textRotation="0" wrapText="0" indent="0" shrinkToFit="0"/>
-      <border>
-        <left style="thin">
-          <color rgb="FF000000"/>
-        </left>
-        <right style="thin">
-          <color rgb="FF000000"/>
-        </right>
-        <top style="thin">
-          <color rgb="FF000000"/>
-        </top>
-        <bottom style="thin">
-          <color rgb="FF000000"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="top" textRotation="0" wrapText="0" indent="0" shrinkToFit="0"/>
-      <border>
-        <left style="thin">
-          <color rgb="FF000000"/>
-        </left>
-        <right style="thin">
-          <color rgb="FF000000"/>
-        </right>
-        <top style="thin">
-          <color rgb="FF000000"/>
-        </top>
-        <bottom style="thin">
-          <color rgb="FF000000"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="top" textRotation="0" wrapText="0" indent="0" shrinkToFit="0"/>
-      <border>
-        <left style="thin">
-          <color rgb="FF000000"/>
-        </left>
-        <right style="thin">
-          <color rgb="FF000000"/>
-        </right>
-        <top style="thin">
-          <color rgb="FF000000"/>
-        </top>
-        <bottom style="thin">
-          <color rgb="FF000000"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-      </font>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="top" textRotation="0" wrapText="0" indent="0" shrinkToFit="0"/>
-      <border>
-        <left style="thin">
-          <color rgb="FF000000"/>
-        </left>
-        <right style="thin">
-          <color rgb="FF000000"/>
-        </right>
-        <top style="thin">
-          <color rgb="FF000000"/>
-        </top>
-        <bottom style="thin">
-          <color rgb="FF000000"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-      </font>
-    </dxf>
-    <dxf>
-      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="1" indent="0" shrinkToFit="0"/>
-      <border>
-        <left style="thin">
-          <color rgb="FF000000"/>
-        </left>
-        <right style="thin">
-          <color rgb="FF000000"/>
-        </right>
-        <top style="thin">
-          <color rgb="FF000000"/>
-        </top>
-        <bottom style="thin">
-          <color rgb="FF000000"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="1" indent="0" shrinkToFit="0"/>
-      <border>
-        <left style="thin">
-          <color rgb="FF000000"/>
-        </left>
-        <right style="thin">
-          <color rgb="FF000000"/>
-        </right>
-        <top style="thin">
-          <color rgb="FF000000"/>
-        </top>
-        <bottom style="thin">
-          <color rgb="FF000000"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="1" indent="0" shrinkToFit="0"/>
-      <border>
-        <left style="thin">
-          <color rgb="FF000000"/>
-        </left>
-        <right style="thin">
-          <color rgb="FF000000"/>
-        </right>
-        <top style="thin">
-          <color rgb="FF000000"/>
-        </top>
-        <bottom style="thin">
-          <color rgb="FF000000"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="1" indent="0" shrinkToFit="0"/>
-      <border>
-        <left style="thin">
-          <color rgb="FF000000"/>
-        </left>
-        <right style="thin">
-          <color rgb="FF000000"/>
-        </right>
-        <top style="thin">
-          <color rgb="FF000000"/>
-        </top>
-        <bottom style="thin">
-          <color rgb="FF000000"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="0" indent="0" shrinkToFit="0"/>
-      <border>
-        <left style="thin">
-          <color rgb="FF000000"/>
-        </left>
-        <right style="thin">
-          <color rgb="FF000000"/>
-        </right>
-        <top style="thin">
-          <color rgb="FF000000"/>
-        </top>
-        <bottom style="thin">
-          <color rgb="FF000000"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="1" indent="0" shrinkToFit="0"/>
-      <border>
-        <left style="thin">
-          <color rgb="FF000000"/>
-        </left>
-        <right style="thin">
-          <color rgb="FF000000"/>
-        </right>
-        <top style="thin">
-          <color rgb="FF000000"/>
-        </top>
-        <bottom style="thin">
-          <color rgb="FF000000"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <alignment vertical="top" textRotation="0" wrapText="0" indent="0" shrinkToFit="0"/>
-      <border>
-        <left style="thin">
-          <color rgb="FF000000"/>
-        </left>
-        <right style="thin">
-          <color rgb="FF000000"/>
-        </right>
-        <top style="thin">
-          <color rgb="FF000000"/>
-        </top>
-        <bottom style="thin">
-          <color rgb="FF000000"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="top" textRotation="0" wrapText="0" indent="0" shrinkToFit="0"/>
-      <border>
-        <left style="thin">
-          <color rgb="FF000000"/>
-        </left>
-        <right style="thin">
-          <color rgb="FF000000"/>
-        </right>
-        <top style="thin">
-          <color rgb="FF000000"/>
-        </top>
-        <bottom style="thin">
-          <color rgb="FF000000"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-      </font>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="top" textRotation="0" wrapText="1" indent="0" shrinkToFit="0"/>
-      <border>
         <left style="thin">
           <color rgb="FF000000"/>
         </left>
@@ -3465,6 +3553,23 @@
       </font>
       <alignment vertical="top" textRotation="0" wrapText="1" indent="0" shrinkToFit="0"/>
       <border>
+        <left style="thin">
+          <color rgb="FF000000"/>
+        </left>
+        <right style="thin">
+          <color rgb="FF000000"/>
+        </right>
+        <top style="thin">
+          <color rgb="FF000000"/>
+        </top>
+        <bottom style="thin">
+          <color rgb="FF000000"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border outline="0">
         <left style="thin">
           <color rgb="FF000000"/>
         </left>
@@ -3510,30 +3615,30 @@
     <sortCondition ref="B2:B8"/>
   </sortState>
   <tableColumns count="17">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Tier" dataDxfId="48"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Full ref" dataDxfId="70"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="1AU" dataDxfId="45"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="Year" dataDxfId="69"/>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="Paper Type" dataDxfId="35"/>
-    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" name="Link" dataDxfId="46"/>
-    <tableColumn id="11" xr3:uid="{00000000-0010-0000-0000-00000B000000}" name="RQ" dataDxfId="26"/>
-    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0000-000008000000}" name="nrParticip" dataDxfId="47"/>
-    <tableColumn id="15" xr3:uid="{00000000-0010-0000-0000-00000F000000}" name="Population" dataDxfId="44"/>
-    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0000-000009000000}" name="Approach" dataDxfId="43"/>
-    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0000-00000A000000}" name="WhatWasMeasured?" dataDxfId="42"/>
-    <tableColumn id="13" xr3:uid="{00000000-0010-0000-0000-00000D000000}" name="MainFinding" dataDxfId="41"/>
-    <tableColumn id="14" xr3:uid="{00000000-0010-0000-0000-00000E000000}" name="Other" dataDxfId="40"/>
-    <tableColumn id="16" xr3:uid="{00000000-0010-0000-0000-000010000000}" name="Orientation" dataDxfId="39"/>
-    <tableColumn id="12" xr3:uid="{00000000-0010-0000-0000-00000C000000}" name="Analysis" dataDxfId="38"/>
-    <tableColumn id="18" xr3:uid="{00000000-0010-0000-0000-000012000000}" name="Country" dataDxfId="36"/>
-    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0000-000007000000}" name="Venues" dataDxfId="37"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Tier" dataDxfId="70"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Full ref" dataDxfId="69"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="1AU" dataDxfId="68"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="Year" dataDxfId="67"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="Paper Type" dataDxfId="66"/>
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" name="Link" dataDxfId="65"/>
+    <tableColumn id="11" xr3:uid="{00000000-0010-0000-0000-00000B000000}" name="RQ" dataDxfId="64"/>
+    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0000-000008000000}" name="nrParticip" dataDxfId="63"/>
+    <tableColumn id="15" xr3:uid="{00000000-0010-0000-0000-00000F000000}" name="Population" dataDxfId="62"/>
+    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0000-000009000000}" name="Approach" dataDxfId="61"/>
+    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0000-00000A000000}" name="WhatWasMeasured?" dataDxfId="60"/>
+    <tableColumn id="13" xr3:uid="{00000000-0010-0000-0000-00000D000000}" name="MainFinding" dataDxfId="59"/>
+    <tableColumn id="14" xr3:uid="{00000000-0010-0000-0000-00000E000000}" name="Other" dataDxfId="58"/>
+    <tableColumn id="16" xr3:uid="{00000000-0010-0000-0000-000010000000}" name="Orientation" dataDxfId="57"/>
+    <tableColumn id="12" xr3:uid="{00000000-0010-0000-0000-00000C000000}" name="Analysis" dataDxfId="56"/>
+    <tableColumn id="18" xr3:uid="{00000000-0010-0000-0000-000012000000}" name="Country" dataDxfId="55"/>
+    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0000-000007000000}" name="Venues" dataDxfId="54"/>
   </tableColumns>
   <tableStyleInfo showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{00000000-000C-0000-FFFF-FFFF01000000}" name="Table134" displayName="Table134" ref="B2:R9" headerRowDxfId="68">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{00000000-000C-0000-FFFF-FFFF01000000}" name="Table134" displayName="Table134" ref="B2:R9" headerRowDxfId="53">
   <autoFilter ref="B2:R9" xr:uid="{00000000-0009-0000-0100-000002000000}">
     <filterColumn colId="9">
       <filters>
@@ -3545,30 +3650,30 @@
     <sortCondition ref="B2:B9"/>
   </sortState>
   <tableColumns count="17">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0100-000001000000}" name="Tier" dataDxfId="67"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0100-000002000000}" name="Full ref" dataDxfId="34"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0100-000003000000}" name="1AU" dataDxfId="66"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0100-000004000000}" name="Year" dataDxfId="31"/>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0100-000005000000}" name="Paper Type" dataDxfId="29"/>
-    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0100-000006000000}" name="Link" dataDxfId="33"/>
-    <tableColumn id="11" xr3:uid="{00000000-0010-0000-0100-00000B000000}" name="RQ" dataDxfId="24"/>
-    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0100-000008000000}" name="nrParticip" dataDxfId="25"/>
-    <tableColumn id="15" xr3:uid="{00000000-0010-0000-0100-00000F000000}" name="Population" dataDxfId="65"/>
-    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0100-000009000000}" name="Approach" dataDxfId="64"/>
-    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0100-00000A000000}" name="WhatWasMeasured?" dataDxfId="63"/>
-    <tableColumn id="13" xr3:uid="{00000000-0010-0000-0100-00000D000000}" name="MainFinding" dataDxfId="62"/>
-    <tableColumn id="14" xr3:uid="{00000000-0010-0000-0100-00000E000000}" name="Other" dataDxfId="61"/>
-    <tableColumn id="16" xr3:uid="{00000000-0010-0000-0100-000010000000}" name="Orientation" dataDxfId="27"/>
-    <tableColumn id="12" xr3:uid="{00000000-0010-0000-0100-00000C000000}" name="Analysis" dataDxfId="60"/>
-    <tableColumn id="18" xr3:uid="{00000000-0010-0000-0100-000012000000}" name="Country" dataDxfId="32"/>
-    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0100-000007000000}" name=" Venues" dataDxfId="30"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0100-000001000000}" name="Tier" dataDxfId="52"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0100-000002000000}" name="Full ref" dataDxfId="51"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0100-000003000000}" name="1AU" dataDxfId="50"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0100-000004000000}" name="Year" dataDxfId="49"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0100-000005000000}" name="Paper Type" dataDxfId="48"/>
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0100-000006000000}" name="Link" dataDxfId="47"/>
+    <tableColumn id="11" xr3:uid="{00000000-0010-0000-0100-00000B000000}" name="RQ" dataDxfId="46"/>
+    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0100-000008000000}" name="nrParticip" dataDxfId="45"/>
+    <tableColumn id="15" xr3:uid="{00000000-0010-0000-0100-00000F000000}" name="Population" dataDxfId="44"/>
+    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0100-000009000000}" name="Approach" dataDxfId="43"/>
+    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0100-00000A000000}" name="WhatWasMeasured?" dataDxfId="42"/>
+    <tableColumn id="13" xr3:uid="{00000000-0010-0000-0100-00000D000000}" name="MainFinding" dataDxfId="41"/>
+    <tableColumn id="14" xr3:uid="{00000000-0010-0000-0100-00000E000000}" name="Other" dataDxfId="40"/>
+    <tableColumn id="16" xr3:uid="{00000000-0010-0000-0100-000010000000}" name="Orientation" dataDxfId="39"/>
+    <tableColumn id="12" xr3:uid="{00000000-0010-0000-0100-00000C000000}" name="Analysis" dataDxfId="38"/>
+    <tableColumn id="18" xr3:uid="{00000000-0010-0000-0100-000012000000}" name="Country" dataDxfId="37"/>
+    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0100-000007000000}" name=" Venues" dataDxfId="36"/>
   </tableColumns>
   <tableStyleInfo showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{00000000-000C-0000-FFFF-FFFF02000000}" name="Table13" displayName="Table13" ref="B2:R7" headerRowDxfId="59">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{00000000-000C-0000-FFFF-FFFF02000000}" name="Table13" displayName="Table13" ref="B2:R7" headerRowDxfId="35">
   <autoFilter ref="B2:R7" xr:uid="{00000000-0009-0000-0100-000003000000}">
     <filterColumn colId="9">
       <filters>
@@ -3580,31 +3685,31 @@
     <sortCondition ref="B2:B7"/>
   </sortState>
   <tableColumns count="17">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0200-000001000000}" name="Tier" dataDxfId="58"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0200-000002000000}" name="Full ref" dataDxfId="22"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0200-000003000000}" name="1AU" dataDxfId="9"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0200-000004000000}" name="Year" dataDxfId="10"/>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0200-000005000000}" name="Paper Type" dataDxfId="19"/>
-    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0200-000006000000}" name="Link" dataDxfId="11"/>
-    <tableColumn id="11" xr3:uid="{00000000-0010-0000-0200-00000B000000}" name="RQ" dataDxfId="8"/>
-    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0200-000008000000}" name="nrParticip" dataDxfId="6"/>
-    <tableColumn id="15" xr3:uid="{00000000-0010-0000-0200-00000F000000}" name="Population" dataDxfId="7"/>
-    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0200-000009000000}" name="Approach" dataDxfId="15"/>
-    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0200-00000A000000}" name="WhatWasMeasured?" dataDxfId="14"/>
-    <tableColumn id="13" xr3:uid="{00000000-0010-0000-0200-00000D000000}" name="MainFinding" dataDxfId="13"/>
-    <tableColumn id="14" xr3:uid="{00000000-0010-0000-0200-00000E000000}" name="Other" dataDxfId="12"/>
-    <tableColumn id="16" xr3:uid="{00000000-0010-0000-0200-000010000000}" name="Orientation" dataDxfId="18"/>
-    <tableColumn id="12" xr3:uid="{00000000-0010-0000-0200-00000C000000}" name="Analysis" dataDxfId="17"/>
-    <tableColumn id="18" xr3:uid="{00000000-0010-0000-0200-000012000000}" name="Country" dataDxfId="21"/>
-    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0200-000007000000}" name="Ｖenues" dataDxfId="16"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0200-000001000000}" name="Tier" dataDxfId="34"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0200-000002000000}" name="Full ref" dataDxfId="33"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0200-000003000000}" name="1AU" dataDxfId="32"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0200-000004000000}" name="Year" dataDxfId="31"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0200-000005000000}" name="Paper Type" dataDxfId="30"/>
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0200-000006000000}" name="Link" dataDxfId="29"/>
+    <tableColumn id="11" xr3:uid="{00000000-0010-0000-0200-00000B000000}" name="RQ" dataDxfId="28"/>
+    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0200-000008000000}" name="nrParticip" dataDxfId="27"/>
+    <tableColumn id="15" xr3:uid="{00000000-0010-0000-0200-00000F000000}" name="Population" dataDxfId="26"/>
+    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0200-000009000000}" name="Approach" dataDxfId="25"/>
+    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0200-00000A000000}" name="WhatWasMeasured?" dataDxfId="24"/>
+    <tableColumn id="13" xr3:uid="{00000000-0010-0000-0200-00000D000000}" name="MainFinding" dataDxfId="23"/>
+    <tableColumn id="14" xr3:uid="{00000000-0010-0000-0200-00000E000000}" name="Other" dataDxfId="22"/>
+    <tableColumn id="16" xr3:uid="{00000000-0010-0000-0200-000010000000}" name="Orientation" dataDxfId="21"/>
+    <tableColumn id="12" xr3:uid="{00000000-0010-0000-0200-00000C000000}" name="Analysis" dataDxfId="20"/>
+    <tableColumn id="18" xr3:uid="{00000000-0010-0000-0200-000012000000}" name="Country" dataDxfId="19"/>
+    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0200-000007000000}" name="Ｖenues" dataDxfId="18"/>
   </tableColumns>
   <tableStyleInfo showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{00000000-000C-0000-FFFF-FFFF03000000}" name="Table1" displayName="Table1" ref="B2:R8" headerRowDxfId="57">
-  <autoFilter ref="B2:R8" xr:uid="{00000000-0009-0000-0100-000004000000}">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{00000000-000C-0000-FFFF-FFFF03000000}" name="Table1" displayName="Table1" ref="B2:R10" headerRowDxfId="17">
+  <autoFilter ref="B2:R10" xr:uid="{00000000-0009-0000-0100-000004000000}">
     <filterColumn colId="9">
       <filters>
         <filter val="Experiment"/>
@@ -3615,23 +3720,23 @@
     <sortCondition ref="B2:B8"/>
   </sortState>
   <tableColumns count="17">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0300-000001000000}" name="Tier" dataDxfId="56"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0300-000002000000}" name="Full ref" dataDxfId="23"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0300-000003000000}" name="1AU" dataDxfId="1"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0300-000004000000}" name="Year" dataDxfId="55"/>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0300-000005000000}" name="Paper Type" dataDxfId="5"/>
-    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0300-000006000000}" name="Link" dataDxfId="54"/>
-    <tableColumn id="11" xr3:uid="{00000000-0010-0000-0300-00000B000000}" name="RQ" dataDxfId="20"/>
-    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0300-000008000000}" name="nrParticip" dataDxfId="4"/>
-    <tableColumn id="15" xr3:uid="{00000000-0010-0000-0300-00000F000000}" name="Population" dataDxfId="53"/>
-    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0300-000009000000}" name="Approach" dataDxfId="2"/>
-    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0300-00000A000000}" name="WhatWasMeasured?" dataDxfId="52"/>
-    <tableColumn id="13" xr3:uid="{00000000-0010-0000-0300-00000D000000}" name="MainFinding" dataDxfId="51"/>
-    <tableColumn id="14" xr3:uid="{00000000-0010-0000-0300-00000E000000}" name="Other" dataDxfId="50"/>
-    <tableColumn id="16" xr3:uid="{00000000-0010-0000-0300-000010000000}" name="Orientation" dataDxfId="0"/>
-    <tableColumn id="12" xr3:uid="{00000000-0010-0000-0300-00000C000000}" name="Analysis" dataDxfId="49"/>
-    <tableColumn id="18" xr3:uid="{00000000-0010-0000-0300-000012000000}" name="Country" dataDxfId="28"/>
-    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0300-000007000000}" name="Venues" dataDxfId="3"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0300-000001000000}" name="Tier" dataDxfId="16"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0300-000002000000}" name="Full ref" dataDxfId="15"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0300-000003000000}" name="1AU" dataDxfId="14"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0300-000004000000}" name="Year" dataDxfId="13"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0300-000005000000}" name="Paper Type" dataDxfId="12"/>
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0300-000006000000}" name="Link" dataDxfId="11"/>
+    <tableColumn id="11" xr3:uid="{00000000-0010-0000-0300-00000B000000}" name="RQ" dataDxfId="10"/>
+    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0300-000008000000}" name="nrParticip" dataDxfId="9"/>
+    <tableColumn id="15" xr3:uid="{00000000-0010-0000-0300-00000F000000}" name="Population" dataDxfId="8"/>
+    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0300-000009000000}" name="Approach" dataDxfId="7"/>
+    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0300-00000A000000}" name="WhatWasMeasured?" dataDxfId="6"/>
+    <tableColumn id="13" xr3:uid="{00000000-0010-0000-0300-00000D000000}" name="MainFinding" dataDxfId="5"/>
+    <tableColumn id="14" xr3:uid="{00000000-0010-0000-0300-00000E000000}" name="Other" dataDxfId="4"/>
+    <tableColumn id="16" xr3:uid="{00000000-0010-0000-0300-000010000000}" name="Orientation" dataDxfId="3"/>
+    <tableColumn id="12" xr3:uid="{00000000-0010-0000-0300-00000C000000}" name="Analysis" dataDxfId="2"/>
+    <tableColumn id="18" xr3:uid="{00000000-0010-0000-0300-000012000000}" name="Country" dataDxfId="1"/>
+    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0300-000007000000}" name="Venues" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -3960,7 +4065,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DFA2DDE8-1724-4D78-9808-03A075ADE618}">
   <dimension ref="A1:GQ12"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="K1" zoomScale="180" zoomScaleNormal="180" workbookViewId="0">
+    <sheetView topLeftCell="K1" zoomScale="180" zoomScaleNormal="180" workbookViewId="0">
       <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="P17" sqref="P17"/>
     </sheetView>
@@ -3968,42 +4073,42 @@
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="3.5" style="10" customWidth="1"/>
-    <col min="2" max="2" width="10.83203125" style="54" customWidth="1"/>
+    <col min="2" max="2" width="10.83203125" style="48" customWidth="1"/>
     <col min="3" max="3" width="52.33203125" style="10" customWidth="1"/>
     <col min="4" max="5" width="10.83203125" style="11" customWidth="1"/>
     <col min="6" max="6" width="30.83203125" style="11" customWidth="1"/>
-    <col min="7" max="7" width="30.83203125" style="63" customWidth="1"/>
-    <col min="8" max="8" width="30.83203125" style="106" customWidth="1"/>
-    <col min="9" max="9" width="30.83203125" style="58" customWidth="1"/>
-    <col min="10" max="10" width="30.83203125" style="70" customWidth="1"/>
-    <col min="11" max="14" width="30.83203125" style="58" customWidth="1"/>
-    <col min="15" max="15" width="10.83203125" style="54" customWidth="1"/>
-    <col min="16" max="16" width="30.83203125" style="54" customWidth="1"/>
-    <col min="17" max="17" width="10.83203125" style="54" customWidth="1"/>
-    <col min="18" max="18" width="30.83203125" style="54" customWidth="1"/>
+    <col min="7" max="7" width="30.83203125" style="57" customWidth="1"/>
+    <col min="8" max="8" width="30.83203125" style="91" customWidth="1"/>
+    <col min="9" max="9" width="30.83203125" style="52" customWidth="1"/>
+    <col min="10" max="10" width="30.83203125" style="64" customWidth="1"/>
+    <col min="11" max="14" width="30.83203125" style="52" customWidth="1"/>
+    <col min="15" max="15" width="10.83203125" style="48" customWidth="1"/>
+    <col min="16" max="16" width="30.83203125" style="48" customWidth="1"/>
+    <col min="17" max="17" width="10.83203125" style="48" customWidth="1"/>
+    <col min="18" max="18" width="30.83203125" style="48" customWidth="1"/>
     <col min="19" max="199" width="9.1640625" style="12" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="2:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B1" s="42" t="s">
+      <c r="B1" s="108" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="43"/>
-      <c r="D1" s="43"/>
-      <c r="E1" s="44"/>
-      <c r="F1" s="43"/>
-      <c r="G1" s="43"/>
-      <c r="H1" s="44"/>
-      <c r="I1" s="44"/>
-      <c r="J1" s="44"/>
-      <c r="K1" s="44"/>
-      <c r="L1" s="44"/>
-      <c r="M1" s="44"/>
-      <c r="N1" s="44"/>
-      <c r="O1" s="44"/>
-      <c r="P1" s="43"/>
-      <c r="Q1" s="43"/>
-      <c r="R1" s="43"/>
+      <c r="C1" s="109"/>
+      <c r="D1" s="109"/>
+      <c r="E1" s="110"/>
+      <c r="F1" s="109"/>
+      <c r="G1" s="109"/>
+      <c r="H1" s="110"/>
+      <c r="I1" s="110"/>
+      <c r="J1" s="110"/>
+      <c r="K1" s="110"/>
+      <c r="L1" s="110"/>
+      <c r="M1" s="110"/>
+      <c r="N1" s="110"/>
+      <c r="O1" s="110"/>
+      <c r="P1" s="109"/>
+      <c r="Q1" s="109"/>
+      <c r="R1" s="109"/>
     </row>
     <row r="2" spans="2:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B2" s="1" t="s">
@@ -4021,28 +4126,28 @@
       <c r="F2" s="1" t="s">
         <v>254</v>
       </c>
-      <c r="G2" s="64" t="s">
+      <c r="G2" s="58" t="s">
         <v>5</v>
       </c>
-      <c r="H2" s="103" t="s">
+      <c r="H2" s="88" t="s">
         <v>6</v>
       </c>
-      <c r="I2" s="55" t="s">
+      <c r="I2" s="49" t="s">
         <v>7</v>
       </c>
-      <c r="J2" s="55" t="s">
+      <c r="J2" s="49" t="s">
         <v>8</v>
       </c>
-      <c r="K2" s="55" t="s">
+      <c r="K2" s="49" t="s">
         <v>9</v>
       </c>
-      <c r="L2" s="71" t="s">
+      <c r="L2" s="65" t="s">
         <v>10</v>
       </c>
-      <c r="M2" s="71" t="s">
+      <c r="M2" s="65" t="s">
         <v>11</v>
       </c>
-      <c r="N2" s="55" t="s">
+      <c r="N2" s="49" t="s">
         <v>12</v>
       </c>
       <c r="O2" s="1" t="s">
@@ -4059,7 +4164,7 @@
       </c>
     </row>
     <row r="3" spans="2:18" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B3" s="50">
+      <c r="B3" s="44">
         <v>1</v>
       </c>
       <c r="C3" s="3" t="s">
@@ -4074,16 +4179,16 @@
       <c r="F3" s="2" t="s">
         <v>271</v>
       </c>
-      <c r="G3" s="60" t="s">
+      <c r="G3" s="54" t="s">
         <v>255</v>
       </c>
-      <c r="H3" s="98" t="s">
+      <c r="H3" s="83" t="s">
         <v>17</v>
       </c>
       <c r="I3" s="13" t="s">
         <v>18</v>
       </c>
-      <c r="J3" s="66" t="s">
+      <c r="J3" s="60" t="s">
         <v>19</v>
       </c>
       <c r="K3" s="13" t="s">
@@ -4098,21 +4203,21 @@
       <c r="N3" s="13" t="s">
         <v>23</v>
       </c>
-      <c r="O3" s="50" t="s">
+      <c r="O3" s="44" t="s">
         <v>187</v>
       </c>
-      <c r="P3" s="50" t="s">
+      <c r="P3" s="44" t="s">
         <v>24</v>
       </c>
-      <c r="Q3" s="50" t="s">
+      <c r="Q3" s="44" t="s">
         <v>25</v>
       </c>
-      <c r="R3" s="50" t="s">
+      <c r="R3" s="44" t="s">
         <v>250</v>
       </c>
     </row>
     <row r="4" spans="2:18" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B4" s="51">
+      <c r="B4" s="45">
         <v>2</v>
       </c>
       <c r="C4" s="5" t="s">
@@ -4127,16 +4232,16 @@
       <c r="F4" s="4" t="s">
         <v>269</v>
       </c>
-      <c r="G4" s="65" t="s">
+      <c r="G4" s="59" t="s">
         <v>256</v>
       </c>
-      <c r="H4" s="99" t="s">
+      <c r="H4" s="84" t="s">
         <v>27</v>
       </c>
       <c r="I4" s="14" t="s">
         <v>28</v>
       </c>
-      <c r="J4" s="67" t="s">
+      <c r="J4" s="61" t="s">
         <v>29</v>
       </c>
       <c r="K4" s="14" t="s">
@@ -4151,21 +4256,21 @@
       <c r="N4" s="14" t="s">
         <v>32</v>
       </c>
-      <c r="O4" s="51" t="s">
+      <c r="O4" s="45" t="s">
         <v>187</v>
       </c>
-      <c r="P4" s="51" t="s">
+      <c r="P4" s="45" t="s">
         <v>33</v>
       </c>
-      <c r="Q4" s="51" t="s">
+      <c r="Q4" s="45" t="s">
         <v>25</v>
       </c>
-      <c r="R4" s="51" t="s">
+      <c r="R4" s="45" t="s">
         <v>34</v>
       </c>
     </row>
     <row r="5" spans="2:18" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B5" s="50">
+      <c r="B5" s="44">
         <v>2</v>
       </c>
       <c r="C5" s="3" t="s">
@@ -4180,14 +4285,14 @@
       <c r="F5" s="2" t="s">
         <v>272</v>
       </c>
-      <c r="G5" s="60" t="s">
+      <c r="G5" s="54" t="s">
         <v>257</v>
       </c>
-      <c r="H5" s="98" t="s">
+      <c r="H5" s="83" t="s">
         <v>36</v>
       </c>
       <c r="I5" s="13"/>
-      <c r="J5" s="66" t="s">
+      <c r="J5" s="60" t="s">
         <v>37</v>
       </c>
       <c r="K5" s="13" t="s">
@@ -4202,21 +4307,21 @@
       <c r="N5" s="13" t="s">
         <v>41</v>
       </c>
-      <c r="O5" s="50" t="s">
+      <c r="O5" s="44" t="s">
         <v>42</v>
       </c>
-      <c r="P5" s="50" t="s">
+      <c r="P5" s="44" t="s">
         <v>43</v>
       </c>
-      <c r="Q5" s="50" t="s">
+      <c r="Q5" s="44" t="s">
         <v>44</v>
       </c>
-      <c r="R5" s="50" t="s">
+      <c r="R5" s="44" t="s">
         <v>251</v>
       </c>
     </row>
     <row r="6" spans="2:18" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B6" s="51" t="s">
+      <c r="B6" s="45" t="s">
         <v>275</v>
       </c>
       <c r="C6" s="5" t="s">
@@ -4231,14 +4336,14 @@
       <c r="F6" s="4" t="s">
         <v>268</v>
       </c>
-      <c r="G6" s="65" t="s">
+      <c r="G6" s="59" t="s">
         <v>258</v>
       </c>
-      <c r="H6" s="99" t="s">
+      <c r="H6" s="84" t="s">
         <v>47</v>
       </c>
       <c r="I6" s="14"/>
-      <c r="J6" s="67" t="s">
+      <c r="J6" s="61" t="s">
         <v>37</v>
       </c>
       <c r="K6" s="14" t="s">
@@ -4253,21 +4358,21 @@
       <c r="N6" s="14" t="s">
         <v>50</v>
       </c>
-      <c r="O6" s="51" t="s">
+      <c r="O6" s="45" t="s">
         <v>51</v>
       </c>
-      <c r="P6" s="51" t="s">
+      <c r="P6" s="45" t="s">
         <v>24</v>
       </c>
-      <c r="Q6" s="51" t="s">
+      <c r="Q6" s="45" t="s">
         <v>25</v>
       </c>
-      <c r="R6" s="51" t="s">
+      <c r="R6" s="45" t="s">
         <v>46</v>
       </c>
     </row>
     <row r="7" spans="2:18" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B7" s="50">
+      <c r="B7" s="44">
         <v>3</v>
       </c>
       <c r="C7" s="3" t="s">
@@ -4282,14 +4387,14 @@
       <c r="F7" s="2" t="s">
         <v>270</v>
       </c>
-      <c r="G7" s="60" t="s">
+      <c r="G7" s="54" t="s">
         <v>259</v>
       </c>
-      <c r="H7" s="98" t="s">
+      <c r="H7" s="83" t="s">
         <v>54</v>
       </c>
       <c r="I7" s="13"/>
-      <c r="J7" s="66" t="s">
+      <c r="J7" s="60" t="s">
         <v>37</v>
       </c>
       <c r="K7" s="13" t="s">
@@ -4304,21 +4409,21 @@
       <c r="N7" s="13" t="s">
         <v>57</v>
       </c>
-      <c r="O7" s="50" t="s">
+      <c r="O7" s="44" t="s">
         <v>42</v>
       </c>
-      <c r="P7" s="50" t="s">
+      <c r="P7" s="44" t="s">
         <v>58</v>
       </c>
-      <c r="Q7" s="50" t="s">
+      <c r="Q7" s="44" t="s">
         <v>59</v>
       </c>
-      <c r="R7" s="50" t="s">
+      <c r="R7" s="44" t="s">
         <v>252</v>
       </c>
     </row>
     <row r="8" spans="2:18" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B8" s="51">
+      <c r="B8" s="45">
         <v>2</v>
       </c>
       <c r="C8" s="5" t="s">
@@ -4333,16 +4438,16 @@
       <c r="F8" s="4" t="s">
         <v>276</v>
       </c>
-      <c r="G8" s="65" t="s">
+      <c r="G8" s="59" t="s">
         <v>260</v>
       </c>
-      <c r="H8" s="99" t="s">
+      <c r="H8" s="84" t="s">
         <v>62</v>
       </c>
       <c r="I8" s="14" t="s">
         <v>63</v>
       </c>
-      <c r="J8" s="67" t="s">
+      <c r="J8" s="61" t="s">
         <v>64</v>
       </c>
       <c r="K8" s="13" t="s">
@@ -4357,21 +4462,21 @@
       <c r="N8" s="14" t="s">
         <v>67</v>
       </c>
-      <c r="O8" s="51" t="s">
+      <c r="O8" s="45" t="s">
         <v>42</v>
       </c>
-      <c r="P8" s="51" t="s">
+      <c r="P8" s="45" t="s">
         <v>69</v>
       </c>
-      <c r="Q8" s="51" t="s">
+      <c r="Q8" s="45" t="s">
         <v>44</v>
       </c>
-      <c r="R8" s="51" t="s">
+      <c r="R8" s="45" t="s">
         <v>61</v>
       </c>
     </row>
     <row r="9" spans="2:18" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B9" s="50">
+      <c r="B9" s="44">
         <v>3</v>
       </c>
       <c r="C9" s="3" t="s">
@@ -4386,14 +4491,14 @@
       <c r="F9" s="2" t="s">
         <v>273</v>
       </c>
-      <c r="G9" s="60" t="s">
+      <c r="G9" s="54" t="s">
         <v>261</v>
       </c>
-      <c r="H9" s="98" t="s">
+      <c r="H9" s="83" t="s">
         <v>73</v>
       </c>
       <c r="I9" s="13"/>
-      <c r="J9" s="66" t="s">
+      <c r="J9" s="60" t="s">
         <v>37</v>
       </c>
       <c r="K9" s="13" t="s">
@@ -4408,21 +4513,21 @@
       <c r="N9" s="13" t="s">
         <v>76</v>
       </c>
-      <c r="O9" s="50" t="s">
+      <c r="O9" s="44" t="s">
         <v>42</v>
       </c>
-      <c r="P9" s="50" t="s">
+      <c r="P9" s="44" t="s">
         <v>77</v>
       </c>
-      <c r="Q9" s="50" t="s">
+      <c r="Q9" s="44" t="s">
         <v>78</v>
       </c>
-      <c r="R9" s="50" t="s">
+      <c r="R9" s="44" t="s">
         <v>72</v>
       </c>
     </row>
     <row r="10" spans="2:18" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B10" s="51">
+      <c r="B10" s="45">
         <v>3</v>
       </c>
       <c r="C10" s="5" t="s">
@@ -4437,16 +4542,16 @@
       <c r="F10" s="4" t="s">
         <v>274</v>
       </c>
-      <c r="G10" s="65" t="s">
+      <c r="G10" s="59" t="s">
         <v>262</v>
       </c>
-      <c r="H10" s="99" t="s">
+      <c r="H10" s="84" t="s">
         <v>265</v>
       </c>
       <c r="I10" s="14" t="s">
         <v>80</v>
       </c>
-      <c r="J10" s="67" t="s">
+      <c r="J10" s="61" t="s">
         <v>81</v>
       </c>
       <c r="K10" s="14" t="s">
@@ -4461,56 +4566,56 @@
       <c r="N10" s="14" t="s">
         <v>82</v>
       </c>
-      <c r="O10" s="51" t="s">
+      <c r="O10" s="45" t="s">
         <v>83</v>
       </c>
-      <c r="P10" s="51" t="s">
+      <c r="P10" s="45" t="s">
         <v>24</v>
       </c>
-      <c r="Q10" s="51" t="s">
+      <c r="Q10" s="45" t="s">
         <v>25</v>
       </c>
-      <c r="R10" s="51" t="s">
+      <c r="R10" s="45" t="s">
         <v>253</v>
       </c>
     </row>
     <row r="11" spans="2:18" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B11" s="52"/>
+      <c r="B11" s="46"/>
       <c r="C11" s="7"/>
       <c r="D11" s="6"/>
       <c r="E11" s="6"/>
       <c r="F11" s="6"/>
-      <c r="G11" s="61"/>
-      <c r="H11" s="104"/>
-      <c r="I11" s="56"/>
-      <c r="J11" s="68"/>
-      <c r="K11" s="56"/>
-      <c r="L11" s="56"/>
-      <c r="M11" s="56"/>
-      <c r="N11" s="56"/>
-      <c r="O11" s="52"/>
-      <c r="P11" s="52"/>
-      <c r="Q11" s="52"/>
-      <c r="R11" s="52"/>
+      <c r="G11" s="55"/>
+      <c r="H11" s="89"/>
+      <c r="I11" s="50"/>
+      <c r="J11" s="62"/>
+      <c r="K11" s="50"/>
+      <c r="L11" s="50"/>
+      <c r="M11" s="50"/>
+      <c r="N11" s="50"/>
+      <c r="O11" s="46"/>
+      <c r="P11" s="46"/>
+      <c r="Q11" s="46"/>
+      <c r="R11" s="46"/>
     </row>
     <row r="12" spans="2:18" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B12" s="53"/>
+      <c r="B12" s="47"/>
       <c r="C12" s="9"/>
       <c r="D12" s="8"/>
       <c r="E12" s="8"/>
       <c r="F12" s="8"/>
-      <c r="G12" s="62"/>
-      <c r="H12" s="105"/>
-      <c r="I12" s="57"/>
-      <c r="J12" s="69"/>
-      <c r="K12" s="57"/>
-      <c r="L12" s="57"/>
-      <c r="M12" s="57"/>
-      <c r="N12" s="57"/>
-      <c r="O12" s="53"/>
-      <c r="P12" s="53"/>
-      <c r="Q12" s="53"/>
-      <c r="R12" s="53"/>
+      <c r="G12" s="56"/>
+      <c r="H12" s="90"/>
+      <c r="I12" s="51"/>
+      <c r="J12" s="63"/>
+      <c r="K12" s="51"/>
+      <c r="L12" s="51"/>
+      <c r="M12" s="51"/>
+      <c r="N12" s="51"/>
+      <c r="O12" s="47"/>
+      <c r="P12" s="47"/>
+      <c r="Q12" s="47"/>
+      <c r="R12" s="47"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -4553,38 +4658,38 @@
     <col min="2" max="2" width="10.83203125" style="20" customWidth="1"/>
     <col min="3" max="3" width="30.83203125" style="10" customWidth="1"/>
     <col min="4" max="4" width="10.83203125" style="21" customWidth="1"/>
-    <col min="5" max="5" width="10.83203125" style="94" customWidth="1"/>
-    <col min="6" max="6" width="30.83203125" style="85" customWidth="1"/>
+    <col min="5" max="5" width="10.83203125" style="20" customWidth="1"/>
+    <col min="6" max="6" width="30.83203125" style="79" customWidth="1"/>
     <col min="7" max="7" width="30.83203125" style="10" customWidth="1"/>
-    <col min="8" max="8" width="30.83203125" style="114" customWidth="1"/>
+    <col min="8" max="8" width="30.83203125" style="99" customWidth="1"/>
     <col min="9" max="10" width="30.83203125" style="11" customWidth="1"/>
     <col min="11" max="14" width="30.83203125" style="20" customWidth="1"/>
-    <col min="15" max="15" width="10.83203125" style="85" customWidth="1"/>
+    <col min="15" max="15" width="10.83203125" style="79" customWidth="1"/>
     <col min="16" max="16" width="30.83203125" style="21" customWidth="1"/>
-    <col min="17" max="17" width="10.83203125" style="85" customWidth="1"/>
-    <col min="18" max="18" width="10.83203125" style="54" customWidth="1"/>
+    <col min="17" max="17" width="10.83203125" style="79" customWidth="1"/>
+    <col min="18" max="18" width="10.83203125" style="48" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="2:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B1" s="45" t="s">
+      <c r="B1" s="111" t="s">
         <v>84</v>
       </c>
-      <c r="C1" s="46"/>
-      <c r="D1" s="46"/>
-      <c r="E1" s="47"/>
-      <c r="F1" s="46"/>
-      <c r="G1" s="46"/>
-      <c r="H1" s="47"/>
-      <c r="I1" s="47"/>
-      <c r="J1" s="44"/>
-      <c r="K1" s="47"/>
-      <c r="L1" s="47"/>
-      <c r="M1" s="47"/>
-      <c r="N1" s="47"/>
-      <c r="O1" s="47"/>
-      <c r="P1" s="46"/>
-      <c r="Q1" s="46"/>
-      <c r="R1" s="46"/>
+      <c r="C1" s="112"/>
+      <c r="D1" s="112"/>
+      <c r="E1" s="113"/>
+      <c r="F1" s="112"/>
+      <c r="G1" s="112"/>
+      <c r="H1" s="113"/>
+      <c r="I1" s="113"/>
+      <c r="J1" s="110"/>
+      <c r="K1" s="113"/>
+      <c r="L1" s="113"/>
+      <c r="M1" s="113"/>
+      <c r="N1" s="113"/>
+      <c r="O1" s="113"/>
+      <c r="P1" s="112"/>
+      <c r="Q1" s="112"/>
+      <c r="R1" s="112"/>
     </row>
     <row r="2" spans="2:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B2" s="15" t="s">
@@ -4596,7 +4701,7 @@
       <c r="D2" s="15" t="s">
         <v>3</v>
       </c>
-      <c r="E2" s="86" t="s">
+      <c r="E2" s="15" t="s">
         <v>4</v>
       </c>
       <c r="F2" s="15" t="s">
@@ -4605,7 +4710,7 @@
       <c r="G2" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="H2" s="111" t="s">
+      <c r="H2" s="96" t="s">
         <v>6</v>
       </c>
       <c r="I2" s="1" t="s">
@@ -4617,10 +4722,10 @@
       <c r="K2" s="15" t="s">
         <v>9</v>
       </c>
-      <c r="L2" s="107" t="s">
+      <c r="L2" s="92" t="s">
         <v>10</v>
       </c>
-      <c r="M2" s="107" t="s">
+      <c r="M2" s="92" t="s">
         <v>11</v>
       </c>
       <c r="N2" s="15" t="s">
@@ -4649,16 +4754,16 @@
       <c r="D3" s="17" t="s">
         <v>86</v>
       </c>
-      <c r="E3" s="87">
+      <c r="E3" s="16">
         <v>2018</v>
       </c>
-      <c r="F3" s="102" t="s">
+      <c r="F3" s="87" t="s">
         <v>295</v>
       </c>
-      <c r="G3" s="59" t="s">
+      <c r="G3" s="53" t="s">
         <v>280</v>
       </c>
-      <c r="H3" s="98" t="s">
+      <c r="H3" s="83" t="s">
         <v>87</v>
       </c>
       <c r="I3" s="2" t="s">
@@ -4679,16 +4784,16 @@
       <c r="N3" s="13" t="s">
         <v>93</v>
       </c>
-      <c r="O3" s="78" t="s">
+      <c r="O3" s="72" t="s">
         <v>83</v>
       </c>
       <c r="P3" s="13" t="s">
         <v>90</v>
       </c>
-      <c r="Q3" s="78" t="s">
+      <c r="Q3" s="72" t="s">
         <v>25</v>
       </c>
-      <c r="R3" s="50" t="s">
+      <c r="R3" s="44" t="s">
         <v>70</v>
       </c>
     </row>
@@ -4702,16 +4807,16 @@
       <c r="D4" s="19" t="s">
         <v>95</v>
       </c>
-      <c r="E4" s="88">
+      <c r="E4" s="18">
         <v>2019</v>
       </c>
-      <c r="F4" s="51" t="s">
+      <c r="F4" s="45" t="s">
         <v>296</v>
       </c>
-      <c r="G4" s="76" t="s">
+      <c r="G4" s="70" t="s">
         <v>279</v>
       </c>
-      <c r="H4" s="99" t="s">
+      <c r="H4" s="84" t="s">
         <v>97</v>
       </c>
       <c r="I4" s="4" t="s">
@@ -4732,16 +4837,16 @@
       <c r="N4" s="14" t="s">
         <v>103</v>
       </c>
-      <c r="O4" s="79" t="s">
+      <c r="O4" s="73" t="s">
         <v>104</v>
       </c>
       <c r="P4" s="14" t="s">
         <v>106</v>
       </c>
-      <c r="Q4" s="79" t="s">
+      <c r="Q4" s="73" t="s">
         <v>25</v>
       </c>
-      <c r="R4" s="51" t="s">
+      <c r="R4" s="45" t="s">
         <v>96</v>
       </c>
     </row>
@@ -4755,16 +4860,16 @@
       <c r="D5" s="17" t="s">
         <v>108</v>
       </c>
-      <c r="E5" s="87">
+      <c r="E5" s="16">
         <v>2023</v>
       </c>
-      <c r="F5" s="50" t="s">
+      <c r="F5" s="44" t="s">
         <v>292</v>
       </c>
-      <c r="G5" s="59" t="s">
+      <c r="G5" s="53" t="s">
         <v>278</v>
       </c>
-      <c r="H5" s="98" t="s">
+      <c r="H5" s="83" t="s">
         <v>110</v>
       </c>
       <c r="I5" s="2" t="s">
@@ -4785,16 +4890,16 @@
       <c r="N5" s="13" t="s">
         <v>116</v>
       </c>
-      <c r="O5" s="78" t="s">
+      <c r="O5" s="72" t="s">
         <v>117</v>
       </c>
       <c r="P5" s="13" t="s">
         <v>287</v>
       </c>
-      <c r="Q5" s="78" t="s">
+      <c r="Q5" s="72" t="s">
         <v>118</v>
       </c>
-      <c r="R5" s="50" t="s">
+      <c r="R5" s="44" t="s">
         <v>109</v>
       </c>
     </row>
@@ -4808,16 +4913,16 @@
       <c r="D6" s="19" t="s">
         <v>281</v>
       </c>
-      <c r="E6" s="88">
+      <c r="E6" s="18">
         <v>2024</v>
       </c>
-      <c r="F6" s="51" t="s">
+      <c r="F6" s="45" t="s">
         <v>293</v>
       </c>
-      <c r="G6" s="76" t="s">
+      <c r="G6" s="70" t="s">
         <v>277</v>
       </c>
-      <c r="H6" s="99" t="s">
+      <c r="H6" s="84" t="s">
         <v>120</v>
       </c>
       <c r="I6" s="4"/>
@@ -4836,16 +4941,16 @@
       <c r="N6" s="14" t="s">
         <v>125</v>
       </c>
-      <c r="O6" s="79" t="s">
+      <c r="O6" s="73" t="s">
         <v>83</v>
       </c>
       <c r="P6" s="14" t="s">
         <v>288</v>
       </c>
-      <c r="Q6" s="79" t="s">
+      <c r="Q6" s="73" t="s">
         <v>44</v>
       </c>
-      <c r="R6" s="51" t="s">
+      <c r="R6" s="45" t="s">
         <v>253</v>
       </c>
     </row>
@@ -4853,25 +4958,25 @@
       <c r="B7" s="26">
         <v>2</v>
       </c>
-      <c r="C7" s="72" t="s">
+      <c r="C7" s="66" t="s">
         <v>282</v>
       </c>
       <c r="D7" s="29" t="s">
         <v>126</v>
       </c>
-      <c r="E7" s="89">
+      <c r="E7" s="26">
         <v>2025</v>
       </c>
-      <c r="F7" s="95" t="s">
+      <c r="F7" s="80" t="s">
         <v>294</v>
       </c>
-      <c r="G7" s="75" t="s">
+      <c r="G7" s="69" t="s">
         <v>283</v>
       </c>
-      <c r="H7" s="115" t="s">
+      <c r="H7" s="100" t="s">
         <v>127</v>
       </c>
-      <c r="I7" s="108" t="s">
+      <c r="I7" s="93" t="s">
         <v>128</v>
       </c>
       <c r="J7" s="34" t="s">
@@ -4889,132 +4994,132 @@
       <c r="N7" s="34" t="s">
         <v>133</v>
       </c>
-      <c r="O7" s="80" t="s">
+      <c r="O7" s="74" t="s">
         <v>291</v>
       </c>
       <c r="P7" s="34" t="s">
         <v>289</v>
       </c>
-      <c r="Q7" s="79" t="s">
+      <c r="Q7" s="73" t="s">
         <v>44</v>
       </c>
-      <c r="R7" s="95" t="s">
+      <c r="R7" s="80" t="s">
         <v>285</v>
       </c>
     </row>
     <row r="8" spans="2:18" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B8" s="27"/>
-      <c r="C8" s="73"/>
+      <c r="C8" s="67"/>
       <c r="D8" s="30"/>
-      <c r="E8" s="90"/>
-      <c r="F8" s="96"/>
+      <c r="E8" s="27"/>
+      <c r="F8" s="81"/>
       <c r="G8" s="32"/>
-      <c r="H8" s="100"/>
-      <c r="I8" s="109"/>
+      <c r="H8" s="85"/>
+      <c r="I8" s="94"/>
       <c r="J8" s="35"/>
       <c r="K8" s="40"/>
       <c r="L8" s="35"/>
       <c r="M8" s="35"/>
       <c r="N8" s="35"/>
-      <c r="O8" s="81"/>
+      <c r="O8" s="75"/>
       <c r="P8" s="35"/>
-      <c r="Q8" s="81"/>
-      <c r="R8" s="96"/>
+      <c r="Q8" s="75"/>
+      <c r="R8" s="81"/>
     </row>
     <row r="9" spans="2:18" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B9" s="28"/>
-      <c r="C9" s="74"/>
+      <c r="C9" s="68"/>
       <c r="D9" s="31"/>
-      <c r="E9" s="91"/>
-      <c r="F9" s="97"/>
+      <c r="E9" s="28"/>
+      <c r="F9" s="82"/>
       <c r="G9" s="33"/>
-      <c r="H9" s="101"/>
-      <c r="I9" s="110"/>
+      <c r="H9" s="86"/>
+      <c r="I9" s="95"/>
       <c r="J9" s="36"/>
       <c r="K9" s="41"/>
       <c r="L9" s="36"/>
       <c r="M9" s="36"/>
       <c r="N9" s="36"/>
-      <c r="O9" s="82"/>
+      <c r="O9" s="76"/>
       <c r="P9" s="36"/>
-      <c r="Q9" s="82"/>
-      <c r="R9" s="97"/>
+      <c r="Q9" s="76"/>
+      <c r="R9" s="82"/>
     </row>
     <row r="10" spans="2:18" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B10" s="22"/>
       <c r="C10" s="7"/>
       <c r="D10" s="23"/>
-      <c r="E10" s="92"/>
-      <c r="F10" s="83"/>
+      <c r="E10" s="22"/>
+      <c r="F10" s="77"/>
       <c r="G10" s="7"/>
-      <c r="H10" s="112"/>
+      <c r="H10" s="97"/>
       <c r="I10" s="6"/>
       <c r="J10" s="6"/>
       <c r="K10" s="22"/>
       <c r="L10" s="22"/>
       <c r="M10" s="22"/>
       <c r="N10" s="22"/>
-      <c r="O10" s="83"/>
+      <c r="O10" s="77"/>
       <c r="P10" s="23"/>
-      <c r="Q10" s="83"/>
-      <c r="R10" s="52"/>
+      <c r="Q10" s="77"/>
+      <c r="R10" s="46"/>
     </row>
     <row r="11" spans="2:18" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B11" s="24"/>
       <c r="C11" s="9"/>
       <c r="D11" s="25"/>
-      <c r="E11" s="93"/>
-      <c r="F11" s="84"/>
+      <c r="E11" s="24"/>
+      <c r="F11" s="78"/>
       <c r="G11" s="9"/>
-      <c r="H11" s="113"/>
+      <c r="H11" s="98"/>
       <c r="I11" s="8"/>
       <c r="J11" s="8"/>
       <c r="K11" s="24"/>
       <c r="L11" s="24"/>
       <c r="M11" s="24"/>
       <c r="N11" s="24"/>
-      <c r="O11" s="84"/>
+      <c r="O11" s="78"/>
       <c r="P11" s="25"/>
-      <c r="Q11" s="84"/>
-      <c r="R11" s="53"/>
+      <c r="Q11" s="78"/>
+      <c r="R11" s="47"/>
     </row>
     <row r="12" spans="2:18" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B12" s="22"/>
       <c r="C12" s="7"/>
       <c r="D12" s="23"/>
-      <c r="E12" s="92"/>
-      <c r="F12" s="83"/>
+      <c r="E12" s="22"/>
+      <c r="F12" s="77"/>
       <c r="G12" s="7"/>
-      <c r="H12" s="112"/>
+      <c r="H12" s="97"/>
       <c r="I12" s="6"/>
       <c r="J12" s="6"/>
       <c r="K12" s="22"/>
       <c r="L12" s="22"/>
       <c r="M12" s="22"/>
       <c r="N12" s="22"/>
-      <c r="O12" s="83"/>
+      <c r="O12" s="77"/>
       <c r="P12" s="23"/>
-      <c r="Q12" s="83"/>
-      <c r="R12" s="52"/>
+      <c r="Q12" s="77"/>
+      <c r="R12" s="46"/>
     </row>
     <row r="13" spans="2:18" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B13" s="24"/>
       <c r="C13" s="9"/>
       <c r="D13" s="25"/>
-      <c r="E13" s="93"/>
-      <c r="F13" s="84"/>
+      <c r="E13" s="24"/>
+      <c r="F13" s="78"/>
       <c r="G13" s="9"/>
-      <c r="H13" s="113"/>
+      <c r="H13" s="98"/>
       <c r="I13" s="8"/>
       <c r="J13" s="8"/>
       <c r="K13" s="24"/>
       <c r="L13" s="24"/>
       <c r="M13" s="24"/>
       <c r="N13" s="24"/>
-      <c r="O13" s="84"/>
+      <c r="O13" s="78"/>
       <c r="P13" s="25"/>
-      <c r="Q13" s="84"/>
-      <c r="R13" s="53"/>
+      <c r="Q13" s="78"/>
+      <c r="R13" s="47"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -5054,40 +5159,40 @@
     <col min="1" max="1" width="3.5" style="21" customWidth="1"/>
     <col min="2" max="2" width="10.83203125" style="20" customWidth="1"/>
     <col min="3" max="3" width="30.83203125" style="10" customWidth="1"/>
-    <col min="4" max="4" width="10.83203125" style="54" customWidth="1"/>
-    <col min="5" max="5" width="10.83203125" style="85" customWidth="1"/>
-    <col min="6" max="6" width="30.83203125" style="54" customWidth="1"/>
-    <col min="7" max="7" width="30.83203125" style="70" customWidth="1"/>
-    <col min="8" max="10" width="30.83203125" style="58" customWidth="1"/>
+    <col min="4" max="4" width="10.83203125" style="48" customWidth="1"/>
+    <col min="5" max="5" width="10.83203125" style="79" customWidth="1"/>
+    <col min="6" max="6" width="30.83203125" style="48" customWidth="1"/>
+    <col min="7" max="7" width="30.83203125" style="64" customWidth="1"/>
+    <col min="8" max="10" width="30.83203125" style="52" customWidth="1"/>
     <col min="11" max="11" width="30.83203125" style="11" customWidth="1"/>
-    <col min="12" max="13" width="30.83203125" style="58" customWidth="1"/>
+    <col min="12" max="13" width="30.83203125" style="52" customWidth="1"/>
     <col min="14" max="14" width="30.83203125" style="11" customWidth="1"/>
-    <col min="15" max="15" width="10.83203125" style="54" customWidth="1"/>
-    <col min="16" max="16" width="30.83203125" style="54" customWidth="1"/>
-    <col min="17" max="17" width="10.83203125" style="54" customWidth="1"/>
+    <col min="15" max="15" width="10.83203125" style="48" customWidth="1"/>
+    <col min="16" max="16" width="30.83203125" style="48" customWidth="1"/>
+    <col min="17" max="17" width="10.83203125" style="48" customWidth="1"/>
     <col min="18" max="18" width="10.83203125" style="10" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="2:18" ht="37.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B1" s="45" t="s">
+      <c r="B1" s="111" t="s">
         <v>134</v>
       </c>
-      <c r="C1" s="46"/>
-      <c r="D1" s="46"/>
-      <c r="E1" s="47"/>
-      <c r="F1" s="46"/>
-      <c r="G1" s="46"/>
-      <c r="H1" s="47"/>
-      <c r="I1" s="47"/>
-      <c r="J1" s="44"/>
-      <c r="K1" s="47"/>
-      <c r="L1" s="47"/>
-      <c r="M1" s="47"/>
-      <c r="N1" s="47"/>
-      <c r="O1" s="47"/>
-      <c r="P1" s="46"/>
-      <c r="Q1" s="46"/>
-      <c r="R1" s="46"/>
+      <c r="C1" s="112"/>
+      <c r="D1" s="112"/>
+      <c r="E1" s="113"/>
+      <c r="F1" s="112"/>
+      <c r="G1" s="112"/>
+      <c r="H1" s="113"/>
+      <c r="I1" s="113"/>
+      <c r="J1" s="110"/>
+      <c r="K1" s="113"/>
+      <c r="L1" s="113"/>
+      <c r="M1" s="113"/>
+      <c r="N1" s="113"/>
+      <c r="O1" s="113"/>
+      <c r="P1" s="112"/>
+      <c r="Q1" s="112"/>
+      <c r="R1" s="112"/>
     </row>
     <row r="2" spans="2:18" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B2" s="15" t="s">
@@ -5105,25 +5210,25 @@
       <c r="F2" s="15" t="s">
         <v>254</v>
       </c>
-      <c r="G2" s="55" t="s">
+      <c r="G2" s="49" t="s">
         <v>5</v>
       </c>
-      <c r="H2" s="55" t="s">
+      <c r="H2" s="49" t="s">
         <v>6</v>
       </c>
-      <c r="I2" s="55" t="s">
+      <c r="I2" s="49" t="s">
         <v>7</v>
       </c>
-      <c r="J2" s="55" t="s">
+      <c r="J2" s="49" t="s">
         <v>8</v>
       </c>
       <c r="K2" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="L2" s="55" t="s">
+      <c r="L2" s="49" t="s">
         <v>10</v>
       </c>
-      <c r="M2" s="55" t="s">
+      <c r="M2" s="49" t="s">
         <v>11</v>
       </c>
       <c r="N2" s="1" t="s">
@@ -5149,16 +5254,16 @@
       <c r="C3" s="3" t="s">
         <v>135</v>
       </c>
-      <c r="D3" s="50" t="s">
+      <c r="D3" s="44" t="s">
         <v>136</v>
       </c>
-      <c r="E3" s="78">
+      <c r="E3" s="72">
         <v>2018</v>
       </c>
-      <c r="F3" s="50" t="s">
+      <c r="F3" s="44" t="s">
         <v>303</v>
       </c>
-      <c r="G3" s="117" t="s">
+      <c r="G3" s="102" t="s">
         <v>304</v>
       </c>
       <c r="H3" s="13" t="s">
@@ -5182,13 +5287,13 @@
       <c r="N3" s="13" t="s">
         <v>143</v>
       </c>
-      <c r="O3" s="50" t="s">
+      <c r="O3" s="44" t="s">
         <v>305</v>
       </c>
-      <c r="P3" s="50" t="s">
+      <c r="P3" s="44" t="s">
         <v>306</v>
       </c>
-      <c r="Q3" s="50" t="s">
+      <c r="Q3" s="44" t="s">
         <v>144</v>
       </c>
       <c r="R3" s="13" t="s">
@@ -5202,16 +5307,16 @@
       <c r="C4" s="5" t="s">
         <v>145</v>
       </c>
-      <c r="D4" s="51" t="s">
+      <c r="D4" s="45" t="s">
         <v>146</v>
       </c>
-      <c r="E4" s="79">
+      <c r="E4" s="73">
         <v>2017</v>
       </c>
-      <c r="F4" s="51" t="s">
+      <c r="F4" s="45" t="s">
         <v>315</v>
       </c>
-      <c r="G4" s="118" t="s">
+      <c r="G4" s="103" t="s">
         <v>297</v>
       </c>
       <c r="H4" s="14" t="s">
@@ -5235,13 +5340,13 @@
       <c r="N4" s="14" t="s">
         <v>152</v>
       </c>
-      <c r="O4" s="51" t="s">
+      <c r="O4" s="45" t="s">
         <v>68</v>
       </c>
-      <c r="P4" s="51" t="s">
+      <c r="P4" s="45" t="s">
         <v>316</v>
       </c>
-      <c r="Q4" s="51" t="s">
+      <c r="Q4" s="45" t="s">
         <v>25</v>
       </c>
       <c r="R4" s="14" t="s">
@@ -5255,16 +5360,16 @@
       <c r="C5" s="3" t="s">
         <v>153</v>
       </c>
-      <c r="D5" s="50" t="s">
+      <c r="D5" s="44" t="s">
         <v>154</v>
       </c>
-      <c r="E5" s="78">
+      <c r="E5" s="72">
         <v>2023</v>
       </c>
-      <c r="F5" s="50" t="s">
+      <c r="F5" s="44" t="s">
         <v>320</v>
       </c>
-      <c r="G5" s="117" t="s">
+      <c r="G5" s="102" t="s">
         <v>298</v>
       </c>
       <c r="H5" s="13" t="s">
@@ -5288,13 +5393,13 @@
       <c r="N5" s="13" t="s">
         <v>161</v>
       </c>
-      <c r="O5" s="50" t="s">
+      <c r="O5" s="44" t="s">
         <v>318</v>
       </c>
-      <c r="P5" s="50" t="s">
+      <c r="P5" s="44" t="s">
         <v>43</v>
       </c>
-      <c r="Q5" s="50" t="s">
+      <c r="Q5" s="44" t="s">
         <v>78</v>
       </c>
       <c r="R5" s="13" t="s">
@@ -5308,16 +5413,16 @@
       <c r="C6" s="5" t="s">
         <v>162</v>
       </c>
-      <c r="D6" s="51" t="s">
+      <c r="D6" s="45" t="s">
         <v>163</v>
       </c>
-      <c r="E6" s="79">
+      <c r="E6" s="73">
         <v>2024</v>
       </c>
-      <c r="F6" s="51" t="s">
+      <c r="F6" s="45" t="s">
         <v>325</v>
       </c>
-      <c r="G6" s="118" t="s">
+      <c r="G6" s="103" t="s">
         <v>299</v>
       </c>
       <c r="H6" s="14" t="s">
@@ -5341,13 +5446,13 @@
       <c r="N6" s="14" t="s">
         <v>169</v>
       </c>
-      <c r="O6" s="51" t="s">
+      <c r="O6" s="45" t="s">
         <v>42</v>
       </c>
-      <c r="P6" s="51" t="s">
+      <c r="P6" s="45" t="s">
         <v>69</v>
       </c>
-      <c r="Q6" s="51" t="s">
+      <c r="Q6" s="45" t="s">
         <v>170</v>
       </c>
       <c r="R6" s="14" t="s">
@@ -5361,16 +5466,16 @@
       <c r="C7" s="3" t="s">
         <v>171</v>
       </c>
-      <c r="D7" s="50" t="s">
+      <c r="D7" s="44" t="s">
         <v>172</v>
       </c>
-      <c r="E7" s="78">
+      <c r="E7" s="72">
         <v>2025</v>
       </c>
-      <c r="F7" s="50" t="s">
+      <c r="F7" s="44" t="s">
         <v>326</v>
       </c>
-      <c r="G7" s="117" t="s">
+      <c r="G7" s="102" t="s">
         <v>301</v>
       </c>
       <c r="H7" s="13" t="s">
@@ -5394,13 +5499,13 @@
       <c r="N7" s="13" t="s">
         <v>178</v>
       </c>
-      <c r="O7" s="50" t="s">
+      <c r="O7" s="44" t="s">
         <v>324</v>
       </c>
-      <c r="P7" s="50" t="s">
+      <c r="P7" s="44" t="s">
         <v>105</v>
       </c>
-      <c r="Q7" s="50" t="s">
+      <c r="Q7" s="44" t="s">
         <v>25</v>
       </c>
       <c r="R7" s="13" t="s">
@@ -5414,16 +5519,16 @@
       <c r="C8" s="3" t="s">
         <v>179</v>
       </c>
-      <c r="D8" s="50" t="s">
+      <c r="D8" s="44" t="s">
         <v>243</v>
       </c>
-      <c r="E8" s="78">
+      <c r="E8" s="72">
         <v>2025</v>
       </c>
-      <c r="F8" s="50" t="s">
+      <c r="F8" s="44" t="s">
         <v>327</v>
       </c>
-      <c r="G8" s="117" t="s">
+      <c r="G8" s="102" t="s">
         <v>300</v>
       </c>
       <c r="H8" s="13" t="s">
@@ -5447,13 +5552,13 @@
       <c r="N8" s="2" t="s">
         <v>186</v>
       </c>
-      <c r="O8" s="50" t="s">
+      <c r="O8" s="44" t="s">
         <v>187</v>
       </c>
-      <c r="P8" s="50" t="s">
+      <c r="P8" s="44" t="s">
         <v>188</v>
       </c>
-      <c r="Q8" s="50" t="s">
+      <c r="Q8" s="44" t="s">
         <v>25</v>
       </c>
       <c r="R8" s="3" t="s">
@@ -5467,16 +5572,16 @@
       <c r="C9" s="5" t="s">
         <v>189</v>
       </c>
-      <c r="D9" s="51" t="s">
+      <c r="D9" s="45" t="s">
         <v>244</v>
       </c>
-      <c r="E9" s="79">
+      <c r="E9" s="73">
         <v>2020</v>
       </c>
-      <c r="F9" s="51" t="s">
+      <c r="F9" s="45" t="s">
         <v>314</v>
       </c>
-      <c r="G9" s="118" t="s">
+      <c r="G9" s="103" t="s">
         <v>302</v>
       </c>
       <c r="H9" s="14" t="s">
@@ -5500,13 +5605,13 @@
       <c r="N9" s="4" t="s">
         <v>313</v>
       </c>
-      <c r="O9" s="51" t="s">
+      <c r="O9" s="45" t="s">
         <v>311</v>
       </c>
-      <c r="P9" s="51" t="s">
+      <c r="P9" s="45" t="s">
         <v>312</v>
       </c>
-      <c r="Q9" s="51" t="s">
+      <c r="Q9" s="45" t="s">
         <v>25</v>
       </c>
       <c r="R9" s="5" t="s">
@@ -5516,39 +5621,39 @@
     <row r="10" spans="2:18" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B10" s="22"/>
       <c r="C10" s="7"/>
-      <c r="D10" s="52"/>
-      <c r="E10" s="83"/>
-      <c r="F10" s="52"/>
-      <c r="G10" s="68"/>
-      <c r="H10" s="56"/>
-      <c r="I10" s="56"/>
-      <c r="J10" s="56"/>
+      <c r="D10" s="46"/>
+      <c r="E10" s="77"/>
+      <c r="F10" s="46"/>
+      <c r="G10" s="62"/>
+      <c r="H10" s="50"/>
+      <c r="I10" s="50"/>
+      <c r="J10" s="50"/>
       <c r="K10" s="6"/>
-      <c r="L10" s="56"/>
-      <c r="M10" s="56"/>
+      <c r="L10" s="50"/>
+      <c r="M10" s="50"/>
       <c r="N10" s="6"/>
-      <c r="O10" s="52"/>
-      <c r="P10" s="52"/>
-      <c r="Q10" s="52"/>
+      <c r="O10" s="46"/>
+      <c r="P10" s="46"/>
+      <c r="Q10" s="46"/>
       <c r="R10" s="7"/>
     </row>
     <row r="11" spans="2:18" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B11" s="24"/>
       <c r="C11" s="9"/>
-      <c r="D11" s="53"/>
-      <c r="E11" s="84"/>
-      <c r="F11" s="53"/>
-      <c r="G11" s="69"/>
-      <c r="H11" s="57"/>
-      <c r="I11" s="57"/>
-      <c r="J11" s="57"/>
+      <c r="D11" s="47"/>
+      <c r="E11" s="78"/>
+      <c r="F11" s="47"/>
+      <c r="G11" s="63"/>
+      <c r="H11" s="51"/>
+      <c r="I11" s="51"/>
+      <c r="J11" s="51"/>
       <c r="K11" s="8"/>
-      <c r="L11" s="57"/>
-      <c r="M11" s="57"/>
+      <c r="L11" s="51"/>
+      <c r="M11" s="51"/>
       <c r="N11" s="8"/>
-      <c r="O11" s="53"/>
-      <c r="P11" s="53"/>
-      <c r="Q11" s="53"/>
+      <c r="O11" s="47"/>
+      <c r="P11" s="47"/>
+      <c r="Q11" s="47"/>
       <c r="R11" s="9"/>
     </row>
   </sheetData>
@@ -5580,9 +5685,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CC5F1699-9B48-80DE-9008-FE191231A1FF}">
   <dimension ref="A1:R12"/>
   <sheetViews>
-    <sheetView topLeftCell="J1" zoomScale="180" zoomScaleNormal="180" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="180" zoomScaleNormal="180" workbookViewId="0">
       <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="P13" sqref="P13"/>
+      <selection pane="bottomLeft" activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -5590,40 +5695,40 @@
     <col min="1" max="1" width="3.5" style="21" customWidth="1"/>
     <col min="2" max="2" width="10.83203125" style="20" customWidth="1"/>
     <col min="3" max="3" width="30.83203125" style="10" customWidth="1"/>
-    <col min="4" max="4" width="10.83203125" style="85" customWidth="1"/>
+    <col min="4" max="4" width="10.83203125" style="79" customWidth="1"/>
     <col min="5" max="5" width="10.83203125" style="20" customWidth="1"/>
-    <col min="6" max="6" width="30.83203125" style="122" customWidth="1"/>
+    <col min="6" max="6" width="30.83203125" style="107" customWidth="1"/>
     <col min="7" max="7" width="30.83203125" style="21" customWidth="1"/>
-    <col min="8" max="8" width="30.83203125" style="114" customWidth="1"/>
+    <col min="8" max="8" width="30.83203125" style="99" customWidth="1"/>
     <col min="9" max="10" width="30.83203125" style="11" customWidth="1"/>
-    <col min="11" max="11" width="30.83203125" style="58" customWidth="1"/>
+    <col min="11" max="11" width="30.83203125" style="52" customWidth="1"/>
     <col min="12" max="14" width="30.83203125" style="20" customWidth="1"/>
     <col min="15" max="15" width="10.83203125" style="20" customWidth="1"/>
     <col min="16" max="16" width="30.83203125" style="21" customWidth="1"/>
-    <col min="17" max="17" width="10.83203125" style="85" customWidth="1"/>
-    <col min="18" max="18" width="10.83203125" style="54" customWidth="1"/>
+    <col min="17" max="17" width="10.83203125" style="79" customWidth="1"/>
+    <col min="18" max="18" width="10.83203125" style="48" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="2:18" ht="37.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B1" s="45" t="s">
+      <c r="B1" s="111" t="s">
         <v>194</v>
       </c>
-      <c r="C1" s="46"/>
-      <c r="D1" s="46"/>
-      <c r="E1" s="47"/>
-      <c r="F1" s="46"/>
-      <c r="G1" s="46"/>
-      <c r="H1" s="47"/>
-      <c r="I1" s="47"/>
-      <c r="J1" s="44"/>
-      <c r="K1" s="47"/>
-      <c r="L1" s="47"/>
-      <c r="M1" s="47"/>
-      <c r="N1" s="47"/>
-      <c r="O1" s="47"/>
-      <c r="P1" s="46"/>
-      <c r="Q1" s="46"/>
-      <c r="R1" s="46"/>
+      <c r="C1" s="112"/>
+      <c r="D1" s="112"/>
+      <c r="E1" s="113"/>
+      <c r="F1" s="112"/>
+      <c r="G1" s="112"/>
+      <c r="H1" s="113"/>
+      <c r="I1" s="113"/>
+      <c r="J1" s="110"/>
+      <c r="K1" s="113"/>
+      <c r="L1" s="113"/>
+      <c r="M1" s="113"/>
+      <c r="N1" s="113"/>
+      <c r="O1" s="113"/>
+      <c r="P1" s="112"/>
+      <c r="Q1" s="112"/>
+      <c r="R1" s="112"/>
     </row>
     <row r="2" spans="2:18" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B2" s="15" t="s">
@@ -5638,13 +5743,13 @@
       <c r="E2" s="15" t="s">
         <v>4</v>
       </c>
-      <c r="F2" s="77" t="s">
+      <c r="F2" s="71" t="s">
         <v>254</v>
       </c>
       <c r="G2" s="15" t="s">
         <v>5</v>
       </c>
-      <c r="H2" s="111" t="s">
+      <c r="H2" s="96" t="s">
         <v>6</v>
       </c>
       <c r="I2" s="1" t="s">
@@ -5653,7 +5758,7 @@
       <c r="J2" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="K2" s="55" t="s">
+      <c r="K2" s="49" t="s">
         <v>9</v>
       </c>
       <c r="L2" s="15" t="s">
@@ -5685,19 +5790,19 @@
       <c r="C3" s="3" t="s">
         <v>195</v>
       </c>
-      <c r="D3" s="78" t="s">
+      <c r="D3" s="72" t="s">
         <v>196</v>
       </c>
       <c r="E3" s="16">
         <v>2023</v>
       </c>
-      <c r="F3" s="48" t="s">
+      <c r="F3" s="42" t="s">
         <v>334</v>
       </c>
-      <c r="G3" s="116" t="s">
+      <c r="G3" s="101" t="s">
         <v>328</v>
       </c>
-      <c r="H3" s="98" t="s">
+      <c r="H3" s="83" t="s">
         <v>197</v>
       </c>
       <c r="I3" s="2"/>
@@ -5722,10 +5827,10 @@
       <c r="P3" s="13" t="s">
         <v>336</v>
       </c>
-      <c r="Q3" s="78" t="s">
+      <c r="Q3" s="72" t="s">
         <v>25</v>
       </c>
-      <c r="R3" s="50" t="s">
+      <c r="R3" s="44" t="s">
         <v>335</v>
       </c>
     </row>
@@ -5736,19 +5841,19 @@
       <c r="C4" s="5" t="s">
         <v>204</v>
       </c>
-      <c r="D4" s="79" t="s">
+      <c r="D4" s="73" t="s">
         <v>338</v>
       </c>
       <c r="E4" s="18">
         <v>2021</v>
       </c>
-      <c r="F4" s="49" t="s">
+      <c r="F4" s="43" t="s">
         <v>337</v>
       </c>
-      <c r="G4" s="119" t="s">
+      <c r="G4" s="104" t="s">
         <v>332</v>
       </c>
-      <c r="H4" s="99" t="s">
+      <c r="H4" s="84" t="s">
         <v>205</v>
       </c>
       <c r="I4" s="4" t="s">
@@ -5775,10 +5880,10 @@
       <c r="P4" s="13" t="s">
         <v>336</v>
       </c>
-      <c r="Q4" s="79" t="s">
+      <c r="Q4" s="73" t="s">
         <v>44</v>
       </c>
-      <c r="R4" s="51" t="s">
+      <c r="R4" s="45" t="s">
         <v>340</v>
       </c>
     </row>
@@ -5789,19 +5894,19 @@
       <c r="C5" s="3" t="s">
         <v>212</v>
       </c>
-      <c r="D5" s="78" t="s">
+      <c r="D5" s="72" t="s">
         <v>213</v>
       </c>
       <c r="E5" s="16">
         <v>2025</v>
       </c>
-      <c r="F5" s="48" t="s">
+      <c r="F5" s="42" t="s">
         <v>341</v>
       </c>
-      <c r="G5" s="116" t="s">
+      <c r="G5" s="101" t="s">
         <v>329</v>
       </c>
-      <c r="H5" s="98" t="s">
+      <c r="H5" s="83" t="s">
         <v>214</v>
       </c>
       <c r="I5" s="2">
@@ -5828,10 +5933,10 @@
       <c r="P5" s="13" t="s">
         <v>220</v>
       </c>
-      <c r="Q5" s="78" t="s">
+      <c r="Q5" s="72" t="s">
         <v>44</v>
       </c>
-      <c r="R5" s="50" t="s">
+      <c r="R5" s="44" t="s">
         <v>342</v>
       </c>
     </row>
@@ -5842,19 +5947,19 @@
       <c r="C6" s="5" t="s">
         <v>221</v>
       </c>
-      <c r="D6" s="79" t="s">
+      <c r="D6" s="73" t="s">
         <v>344</v>
       </c>
       <c r="E6" s="18">
         <v>2021</v>
       </c>
-      <c r="F6" s="49" t="s">
+      <c r="F6" s="43" t="s">
         <v>343</v>
       </c>
-      <c r="G6" s="119" t="s">
+      <c r="G6" s="104" t="s">
         <v>330</v>
       </c>
-      <c r="H6" s="99" t="s">
+      <c r="H6" s="84" t="s">
         <v>222</v>
       </c>
       <c r="I6" s="4" t="s">
@@ -5881,10 +5986,10 @@
       <c r="P6" s="14" t="s">
         <v>349</v>
       </c>
-      <c r="Q6" s="79" t="s">
+      <c r="Q6" s="73" t="s">
         <v>144</v>
       </c>
-      <c r="R6" s="51" t="s">
+      <c r="R6" s="45" t="s">
         <v>350</v>
       </c>
     </row>
@@ -5895,19 +6000,19 @@
       <c r="C7" s="3" t="s">
         <v>225</v>
       </c>
-      <c r="D7" s="78" t="s">
+      <c r="D7" s="72" t="s">
         <v>352</v>
       </c>
       <c r="E7" s="16">
         <v>2022</v>
       </c>
-      <c r="F7" s="48" t="s">
+      <c r="F7" s="42" t="s">
         <v>351</v>
       </c>
-      <c r="G7" s="116" t="s">
+      <c r="G7" s="101" t="s">
         <v>331</v>
       </c>
-      <c r="H7" s="98" t="s">
+      <c r="H7" s="83" t="s">
         <v>226</v>
       </c>
       <c r="I7" s="2" t="s">
@@ -5934,10 +6039,10 @@
       <c r="P7" s="13" t="s">
         <v>232</v>
       </c>
-      <c r="Q7" s="78" t="s">
+      <c r="Q7" s="72" t="s">
         <v>44</v>
       </c>
-      <c r="R7" s="50" t="s">
+      <c r="R7" s="44" t="s">
         <v>355</v>
       </c>
     </row>
@@ -5948,19 +6053,19 @@
       <c r="C8" s="5" t="s">
         <v>233</v>
       </c>
-      <c r="D8" s="79" t="s">
+      <c r="D8" s="73" t="s">
         <v>357</v>
       </c>
       <c r="E8" s="18">
         <v>2023</v>
       </c>
-      <c r="F8" s="51" t="s">
+      <c r="F8" s="45" t="s">
         <v>356</v>
       </c>
-      <c r="G8" s="119" t="s">
+      <c r="G8" s="104" t="s">
         <v>333</v>
       </c>
-      <c r="H8" s="99" t="s">
+      <c r="H8" s="84" t="s">
         <v>234</v>
       </c>
       <c r="I8" s="4"/>
@@ -5985,88 +6090,122 @@
       <c r="P8" s="13" t="s">
         <v>336</v>
       </c>
-      <c r="Q8" s="79" t="s">
+      <c r="Q8" s="73" t="s">
         <v>240</v>
       </c>
-      <c r="R8" s="51" t="s">
+      <c r="R8" s="45" t="s">
         <v>358</v>
       </c>
     </row>
     <row r="9" spans="2:18" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B9" s="22"/>
-      <c r="C9" s="7"/>
-      <c r="D9" s="83"/>
-      <c r="E9" s="22"/>
-      <c r="F9" s="120"/>
-      <c r="G9" s="23"/>
-      <c r="H9" s="112"/>
-      <c r="I9" s="6"/>
-      <c r="J9" s="6"/>
-      <c r="K9" s="56"/>
-      <c r="L9" s="22"/>
-      <c r="M9" s="22"/>
-      <c r="N9" s="22"/>
-      <c r="O9" s="22"/>
-      <c r="P9" s="23"/>
-      <c r="Q9" s="83"/>
-      <c r="R9" s="52"/>
+      <c r="B9" s="114"/>
+      <c r="C9" s="115"/>
+      <c r="D9" s="116"/>
+      <c r="E9" s="114"/>
+      <c r="F9" s="117"/>
+      <c r="G9" s="118"/>
+      <c r="H9" s="119"/>
+      <c r="I9" s="120"/>
+      <c r="J9" s="121"/>
+      <c r="K9" s="121"/>
+      <c r="L9" s="121"/>
+      <c r="M9" s="121"/>
+      <c r="N9" s="121"/>
+      <c r="O9" s="114"/>
+      <c r="P9" s="121"/>
+      <c r="Q9" s="116"/>
+      <c r="R9" s="122"/>
     </row>
-    <row r="10" spans="2:18" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B10" s="24"/>
-      <c r="C10" s="9"/>
-      <c r="D10" s="84"/>
-      <c r="E10" s="24"/>
-      <c r="F10" s="121"/>
-      <c r="G10" s="25"/>
-      <c r="H10" s="113"/>
-      <c r="I10" s="8"/>
-      <c r="J10" s="8"/>
-      <c r="K10" s="57"/>
-      <c r="L10" s="24"/>
-      <c r="M10" s="24"/>
-      <c r="N10" s="24"/>
-      <c r="O10" s="24"/>
-      <c r="P10" s="25"/>
-      <c r="Q10" s="84"/>
-      <c r="R10" s="53"/>
+    <row r="10" spans="2:18" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B10" s="123">
+        <v>2</v>
+      </c>
+      <c r="C10" s="132" t="s">
+        <v>359</v>
+      </c>
+      <c r="D10" s="124" t="s">
+        <v>360</v>
+      </c>
+      <c r="E10" s="123">
+        <v>2024</v>
+      </c>
+      <c r="F10" s="125" t="s">
+        <v>361</v>
+      </c>
+      <c r="G10" s="126" t="s">
+        <v>362</v>
+      </c>
+      <c r="H10" s="127" t="s">
+        <v>363</v>
+      </c>
+      <c r="I10" s="128" t="s">
+        <v>364</v>
+      </c>
+      <c r="J10" s="129" t="s">
+        <v>365</v>
+      </c>
+      <c r="K10" s="129" t="s">
+        <v>366</v>
+      </c>
+      <c r="L10" s="129" t="s">
+        <v>367</v>
+      </c>
+      <c r="M10" s="129" t="s">
+        <v>368</v>
+      </c>
+      <c r="N10" s="129" t="s">
+        <v>369</v>
+      </c>
+      <c r="O10" s="130" t="s">
+        <v>211</v>
+      </c>
+      <c r="P10" s="129" t="s">
+        <v>370</v>
+      </c>
+      <c r="Q10" s="124" t="s">
+        <v>371</v>
+      </c>
+      <c r="R10" s="131" t="s">
+        <v>372</v>
+      </c>
     </row>
     <row r="11" spans="2:18" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B11" s="22"/>
       <c r="C11" s="7"/>
-      <c r="D11" s="83"/>
+      <c r="D11" s="77"/>
       <c r="E11" s="22"/>
-      <c r="F11" s="120"/>
+      <c r="F11" s="105"/>
       <c r="G11" s="23"/>
-      <c r="H11" s="112"/>
+      <c r="H11" s="97"/>
       <c r="I11" s="6"/>
       <c r="J11" s="6"/>
-      <c r="K11" s="56"/>
+      <c r="K11" s="50"/>
       <c r="L11" s="22"/>
       <c r="M11" s="22"/>
       <c r="N11" s="22"/>
       <c r="O11" s="22"/>
       <c r="P11" s="23"/>
-      <c r="Q11" s="83"/>
-      <c r="R11" s="52"/>
+      <c r="Q11" s="77"/>
+      <c r="R11" s="46"/>
     </row>
     <row r="12" spans="2:18" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B12" s="24"/>
       <c r="C12" s="9"/>
-      <c r="D12" s="84"/>
+      <c r="D12" s="78"/>
       <c r="E12" s="24"/>
-      <c r="F12" s="121"/>
+      <c r="F12" s="106"/>
       <c r="G12" s="25"/>
-      <c r="H12" s="113"/>
+      <c r="H12" s="98"/>
       <c r="I12" s="8"/>
       <c r="J12" s="8"/>
-      <c r="K12" s="57"/>
+      <c r="K12" s="51"/>
       <c r="L12" s="24"/>
       <c r="M12" s="24"/>
       <c r="N12" s="24"/>
       <c r="O12" s="24"/>
       <c r="P12" s="25"/>
-      <c r="Q12" s="84"/>
-      <c r="R12" s="53"/>
+      <c r="Q12" s="78"/>
+      <c r="R12" s="47"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -6079,6 +6218,7 @@
     <hyperlink ref="G7" r:id="rId4" xr:uid="{A54671A0-BB8E-174A-9B13-EA1E5832C724}"/>
     <hyperlink ref="G4" r:id="rId5" xr:uid="{0FA30C79-86B4-C345-8FE1-4A42C69B4ADE}"/>
     <hyperlink ref="G8" r:id="rId6" xr:uid="{0DD72D4F-6547-BC41-BDD9-EB28D9A733C3}"/>
+    <hyperlink ref="G10" r:id="rId7" xr:uid="{BAEA3393-68B2-F947-A76B-06A8C622DE57}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait"/>
@@ -6087,7 +6227,7 @@
     <oddFooter>&amp;L&amp;C&amp;R</oddFooter>
   </headerFooter>
   <tableParts count="1">
-    <tablePart r:id="rId7"/>
+    <tablePart r:id="rId8"/>
   </tableParts>
 </worksheet>
 </file>
</xml_diff>